<commit_message>
Commit: Models:created / Migrations:created / Tables:created
</commit_message>
<xml_diff>
--- a/documentation/Expense_Tracker_App_plan.xlsx
+++ b/documentation/Expense_Tracker_App_plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ct08284/sei/projects/deere-project2-starter/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92A2E56-DA21-B441-A50B-37A9EA635AAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D58AF90B-4939-1442-962F-4E037B22D3D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" xr2:uid="{05595CE3-5133-A840-8AB2-952878BB912B}"/>
   </bookViews>
@@ -16,7 +16,8 @@
     <sheet name="Development_plan" sheetId="2" r:id="rId1"/>
     <sheet name="MVP features" sheetId="1" r:id="rId2"/>
     <sheet name="RESTFUL routing" sheetId="5" r:id="rId3"/>
-    <sheet name="Resources" sheetId="3" r:id="rId4"/>
+    <sheet name="Table definitions" sheetId="6" r:id="rId4"/>
+    <sheet name="Resources" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="254">
   <si>
     <t>Feature #</t>
   </si>
@@ -272,39 +273,10 @@
     <t>Create folders</t>
   </si>
   <si>
-    <t>npx sequelize model:generate --name ModelName --attributes: name1:dataType,name2:dataType,name3:dataType</t>
-  </si>
-  <si>
-    <t>models/ModelName.js
-migrations/timestamp-create-ModelName.js</t>
-  </si>
-  <si>
-    <t>Create tables</t>
-  </si>
-  <si>
     <t>npx sequelize db:migrate</t>
   </si>
   <si>
-    <t>Create tables (Uppercase and plural)</t>
-  </si>
-  <si>
     <t>Resources</t>
-  </si>
-  <si>
-    <t>Crete seeders</t>
-  </si>
-  <si>
-    <t>npx sequelize seed:generate --name demo-fruits</t>
-  </si>
-  <si>
-    <t>seeders/timestamp-demo-fruits</t>
-  </si>
-  <si>
-    <t>Import seeders' data</t>
-  </si>
-  <si>
-    <t>1 - Will import ALL seeders
-2 - Will import only the specified file</t>
   </si>
   <si>
     <t>(1) sequelize db:seed:all
@@ -594,13 +566,267 @@
     <t>res.render("index.ejs", {
       expenseIndex: expense,
     });</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>accountId</t>
+  </si>
+  <si>
+    <t>Column</t>
+  </si>
+  <si>
+    <t>DataType</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Is PK?</t>
+  </si>
+  <si>
+    <t>Is FK?</t>
+  </si>
+  <si>
+    <t>Is Unique?</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Varchar</t>
+  </si>
+  <si>
+    <t>Is Null?</t>
+  </si>
+  <si>
+    <t>Accounts</t>
+  </si>
+  <si>
+    <t>Subaccounts</t>
+  </si>
+  <si>
+    <t>PaymentTypes</t>
+  </si>
+  <si>
+    <t>Expenses</t>
+  </si>
+  <si>
+    <t>Money</t>
+  </si>
+  <si>
+    <t>Default value?</t>
+  </si>
+  <si>
+    <t>new Date()</t>
+  </si>
+  <si>
+    <t>Pending expense description</t>
+  </si>
+  <si>
+    <t>Create Account model</t>
+  </si>
+  <si>
+    <t>models/account.js
+migrations/timestamp-create-account.js</t>
+  </si>
+  <si>
+    <t>Create Subaccount model</t>
+  </si>
+  <si>
+    <t>models/subaccount.js
+migrations/timestamp-create-subaccount.js</t>
+  </si>
+  <si>
+    <t>Create PaymentType model</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>Create Status model</t>
+  </si>
+  <si>
+    <t>Create Expense model</t>
+  </si>
+  <si>
+    <t>models/paymenttype.js
+migrations/timestamp-create-payment-type.js</t>
+  </si>
+  <si>
+    <t>models/status.js
+migrations/timestamp-create-status.js</t>
+  </si>
+  <si>
+    <t>models/expense.js
+migrations/timestamp-create-expense.js</t>
+  </si>
+  <si>
+    <t>Update Account model</t>
+  </si>
+  <si>
+    <t>Update Subaccount model</t>
+  </si>
+  <si>
+    <t>Update PaymentType model</t>
+  </si>
+  <si>
+    <t>Update Status model</t>
+  </si>
+  <si>
+    <t>Update Expense model</t>
+  </si>
+  <si>
+    <t>npx sequelize model:generate --name ModelName --attributes: name1:dataType,…</t>
+  </si>
+  <si>
+    <t>migrations/timestamp-create-account.js</t>
+  </si>
+  <si>
+    <t>migrations/timestamp-create-subaccount.js</t>
+  </si>
+  <si>
+    <t>migrations/timestamp-create-status.js</t>
+  </si>
+  <si>
+    <t>migrations/timestamp-create-expense.js</t>
+  </si>
+  <si>
+    <t>"Pending description"</t>
+  </si>
+  <si>
+    <t>Update models and create tables</t>
+  </si>
+  <si>
+    <t>Create Accounts table</t>
+  </si>
+  <si>
+    <t>Update Account migration</t>
+  </si>
+  <si>
+    <t>models/account.js</t>
+  </si>
+  <si>
+    <t>createdAt</t>
+  </si>
+  <si>
+    <t>updatedAt</t>
+  </si>
+  <si>
+    <t>Date timestamp</t>
+  </si>
+  <si>
+    <t>Create Subaccounts table</t>
+  </si>
+  <si>
+    <t>models/Subaccount.js</t>
+  </si>
+  <si>
+    <t>Check table with pgAdmin</t>
+  </si>
+  <si>
+    <t>Update PaymentType migration</t>
+  </si>
+  <si>
+    <t>Create PaymentTypes table</t>
+  </si>
+  <si>
+    <t>Update Status migration</t>
+  </si>
+  <si>
+    <t>models/Status.js</t>
+  </si>
+  <si>
+    <t>Create Statuses table</t>
+  </si>
+  <si>
+    <t>Update Expense migration</t>
+  </si>
+  <si>
+    <t>Create Expenses table</t>
+  </si>
+  <si>
+    <t>models/Expense.js</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>userId</t>
+  </si>
+  <si>
+    <t>https://medium.com/@andrewoons/how-to-define-sequelize-associations-using-migrations-de4333bf75a7</t>
+  </si>
+  <si>
+    <t>Create Seeders</t>
+  </si>
+  <si>
+    <t>Create seeder for Accounts table</t>
+  </si>
+  <si>
+    <t>Create seeder for Subccounts table</t>
+  </si>
+  <si>
+    <t>Import seeders into the table</t>
+  </si>
+  <si>
+    <t>Create seeder for PaymentTypes table</t>
+  </si>
+  <si>
+    <t>Create seeder for Statuses table</t>
+  </si>
+  <si>
+    <t>npx sequelize seed:generate --name demo-accounts</t>
+  </si>
+  <si>
+    <t>npx sequelize seed:generate --name demo-subaccounts</t>
+  </si>
+  <si>
+    <t>npx sequelize seed:generate --name demo-paymentTypes</t>
+  </si>
+  <si>
+    <t>npx sequelize seed:generate --name demo-statuses</t>
+  </si>
+  <si>
+    <t>seeders/timestamp-demo-accounts.js</t>
+  </si>
+  <si>
+    <t>fontColor</t>
+  </si>
+  <si>
+    <t>backgroudColor</t>
+  </si>
+  <si>
+    <t>subaccountId</t>
+  </si>
+  <si>
+    <t>paymentTypeId</t>
+  </si>
+  <si>
+    <t>statusId</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -657,8 +883,16 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -695,8 +929,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -704,12 +962,62 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -757,13 +1065,55 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="1" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1081,18 +1431,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FFC9C39-9695-8A40-8D81-C0586B568F96}">
-  <dimension ref="A1:G98"/>
+  <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23:F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.1640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="36.1640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="38.1640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="15.33203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="46.1640625" style="1" bestFit="1" customWidth="1"/>
@@ -1119,7 +1469,7 @@
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -1134,7 +1484,7 @@
         <v>44043</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -1149,7 +1499,7 @@
         <v>44043</v>
       </c>
       <c r="F3" s="22" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -1164,10 +1514,10 @@
         <v>44044</v>
       </c>
       <c r="F4" s="22" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -1182,10 +1532,10 @@
         <v>44044</v>
       </c>
       <c r="F5" s="22" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1196,13 +1546,13 @@
         <v>70</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="E6" s="6">
         <v>44044</v>
       </c>
-      <c r="F6" s="23" t="s">
-        <v>96</v>
+      <c r="F6" s="32" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -1210,22 +1560,22 @@
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="E7" s="6">
         <v>44045</v>
       </c>
-      <c r="F7" s="23" t="s">
-        <v>96</v>
+      <c r="F7" s="22" t="s">
+        <v>86</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1244,8 +1594,8 @@
       <c r="E8" s="6">
         <v>44045</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>97</v>
+      <c r="F8" s="22" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1264,218 +1614,634 @@
       <c r="E9" s="6">
         <v>44045</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>97</v>
+      <c r="F9" s="22" t="s">
+        <v>86</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="33">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E10" s="6">
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="35">
         <v>44045</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="F10" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>10</v>
+        <v>9.1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>84</v>
+        <v>192</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>85</v>
+        <v>209</v>
       </c>
       <c r="D11" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="22" t="s">
         <v>86</v>
-      </c>
-      <c r="E11" s="6">
-        <v>44045</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>11</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E12" s="6">
-        <v>44045</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>97</v>
+        <v>194</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="22" t="s">
+        <v>86</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>12</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>89</v>
-      </c>
+        <v>196</v>
+      </c>
+      <c r="C13" s="4"/>
       <c r="D13" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="E13" s="6">
-        <v>44045</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>97</v>
+        <v>201</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="22" t="s">
+        <v>86</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="7">
+    <row r="14" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>9.4</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="E14" s="6"/>
+      <c r="F14" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>9.5</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="E15" s="6"/>
+      <c r="F15" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="39">
+        <v>10</v>
+      </c>
+      <c r="B16" s="33" t="s">
+        <v>215</v>
+      </c>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="35">
+        <v>44045</v>
+      </c>
+      <c r="F16" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="G16" s="5"/>
+    </row>
+    <row r="17" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="37">
+        <v>10.1</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="E17" s="6"/>
+      <c r="F17" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>10.11</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="E18" s="6"/>
+      <c r="F18" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>10.119999999999999</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="E19" s="6"/>
+      <c r="F19" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="37">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="E20" s="6"/>
+      <c r="F20" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>10.210000000000001</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="E21" s="6"/>
+      <c r="F21" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>10.220000000000001</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="E22" s="6"/>
+      <c r="F22" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="37">
+        <v>10.3</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="E23" s="6"/>
+      <c r="F23" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>10.31</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="E24" s="6"/>
+      <c r="F24" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>10.32</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="E25" s="6"/>
+      <c r="F25" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="37">
+        <v>10.4</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="E26" s="6"/>
+      <c r="F26" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>10.41</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="E27" s="6"/>
+      <c r="F27" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>10.42</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="E28" s="6"/>
+      <c r="F28" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="37">
+        <v>10.5</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="E29" s="6"/>
+      <c r="F29" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>10.51</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="E30" s="6"/>
+      <c r="F30" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>10.52</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="E31" s="6"/>
+      <c r="F31" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="39">
+        <v>11</v>
+      </c>
+      <c r="B32" s="33" t="s">
+        <v>238</v>
+      </c>
+      <c r="C32" s="34"/>
+      <c r="D32" s="34"/>
+      <c r="E32" s="35">
+        <v>44045</v>
+      </c>
+      <c r="F32" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="40">
+        <v>11.1</v>
+      </c>
+      <c r="B33" s="21" t="s">
+        <v>239</v>
+      </c>
+      <c r="C33" s="41" t="s">
+        <v>244</v>
+      </c>
+      <c r="D33" s="41" t="s">
+        <v>248</v>
+      </c>
+      <c r="E33" s="42"/>
+      <c r="F33" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="G33" s="44"/>
+    </row>
+    <row r="34" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A34" s="40">
+        <v>11.11</v>
+      </c>
+      <c r="B34" s="21" t="s">
+        <v>241</v>
+      </c>
+      <c r="C34" s="41" t="s">
+        <v>80</v>
+      </c>
+      <c r="D34" s="41"/>
+      <c r="E34" s="42"/>
+      <c r="F34" s="43"/>
+      <c r="G34" s="44"/>
+    </row>
+    <row r="35" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" s="40">
+        <v>11.2</v>
+      </c>
+      <c r="B35" s="21" t="s">
+        <v>240</v>
+      </c>
+      <c r="C35" s="41" t="s">
+        <v>245</v>
+      </c>
+      <c r="D35" s="41"/>
+      <c r="E35" s="42"/>
+      <c r="F35" s="43"/>
+      <c r="G35" s="44"/>
+    </row>
+    <row r="36" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A36" s="40">
+        <v>11.21</v>
+      </c>
+      <c r="B36" s="21" t="s">
+        <v>241</v>
+      </c>
+      <c r="C36" s="41" t="s">
+        <v>80</v>
+      </c>
+      <c r="D36" s="41"/>
+      <c r="E36" s="42"/>
+      <c r="F36" s="43"/>
+      <c r="G36" s="44"/>
+    </row>
+    <row r="37" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" s="40">
+        <v>11.3</v>
+      </c>
+      <c r="B37" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="C37" s="41" t="s">
+        <v>246</v>
+      </c>
+      <c r="D37" s="41"/>
+      <c r="E37" s="42"/>
+      <c r="F37" s="43"/>
+      <c r="G37" s="44"/>
+    </row>
+    <row r="38" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A38" s="40">
+        <v>11.31</v>
+      </c>
+      <c r="B38" s="21" t="s">
+        <v>241</v>
+      </c>
+      <c r="C38" s="41" t="s">
+        <v>80</v>
+      </c>
+      <c r="D38" s="41"/>
+      <c r="E38" s="42"/>
+      <c r="F38" s="43"/>
+      <c r="G38" s="44"/>
+    </row>
+    <row r="39" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A39" s="40">
+        <v>11.4</v>
+      </c>
+      <c r="B39" s="21" t="s">
+        <v>243</v>
+      </c>
+      <c r="C39" s="41" t="s">
+        <v>247</v>
+      </c>
+      <c r="D39" s="41"/>
+      <c r="E39" s="42"/>
+      <c r="F39" s="43"/>
+      <c r="G39" s="44"/>
+    </row>
+    <row r="40" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A40" s="40">
+        <v>11.41</v>
+      </c>
+      <c r="B40" s="21" t="s">
+        <v>241</v>
+      </c>
+      <c r="C40" s="41" t="s">
+        <v>80</v>
+      </c>
+      <c r="D40" s="41"/>
+      <c r="E40" s="42"/>
+      <c r="F40" s="43"/>
+      <c r="G40" s="44"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" s="7">
         <v>13</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="9">
+      <c r="B41" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C41" s="8"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="9">
         <v>44045</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C15" s="4"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C16" s="4"/>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C17" s="4"/>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C18" s="4"/>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C19" s="4"/>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C20" s="4"/>
-    </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C21" s="4"/>
-    </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C22" s="4"/>
-    </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C23" s="4"/>
-    </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C24" s="4"/>
-    </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C25" s="4"/>
-    </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C26" s="4"/>
-    </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C27" s="4"/>
-    </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C28" s="4"/>
-    </row>
-    <row r="29" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C29" s="4"/>
-    </row>
-    <row r="30" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C30" s="4"/>
-    </row>
-    <row r="31" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C31" s="4"/>
-    </row>
-    <row r="32" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C32" s="4"/>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C33" s="4"/>
-    </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C34" s="4"/>
-    </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C35" s="4"/>
-    </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C36" s="4"/>
-    </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C37" s="4"/>
-    </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C38" s="4"/>
-    </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C39" s="4"/>
-    </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C40" s="4"/>
-    </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C41" s="4"/>
-    </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C42" s="4"/>
     </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C43" s="4"/>
     </row>
-    <row r="44" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C44" s="4"/>
     </row>
-    <row r="45" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C45" s="4"/>
     </row>
-    <row r="46" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C46" s="4"/>
     </row>
-    <row r="47" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C47" s="4"/>
     </row>
-    <row r="48" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C48" s="4"/>
     </row>
     <row r="49" spans="3:3" x14ac:dyDescent="0.2">
@@ -1627,12 +2393,95 @@
     </row>
     <row r="98" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C98" s="4"/>
+    </row>
+    <row r="99" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C99" s="4"/>
+    </row>
+    <row r="100" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C100" s="4"/>
+    </row>
+    <row r="101" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C101" s="4"/>
+    </row>
+    <row r="102" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C102" s="4"/>
+    </row>
+    <row r="103" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C103" s="4"/>
+    </row>
+    <row r="104" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C104" s="4"/>
+    </row>
+    <row r="105" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C105" s="4"/>
+    </row>
+    <row r="106" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C106" s="4"/>
+    </row>
+    <row r="107" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C107" s="4"/>
+    </row>
+    <row r="108" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C108" s="4"/>
+    </row>
+    <row r="109" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C109" s="4"/>
+    </row>
+    <row r="110" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C110" s="4"/>
+    </row>
+    <row r="111" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C111" s="4"/>
+    </row>
+    <row r="112" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C112" s="4"/>
+    </row>
+    <row r="113" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C113" s="4"/>
+    </row>
+    <row r="114" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C114" s="4"/>
+    </row>
+    <row r="115" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C115" s="4"/>
+    </row>
+    <row r="116" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C116" s="4"/>
+    </row>
+    <row r="117" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C117" s="4"/>
+    </row>
+    <row r="118" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C118" s="4"/>
+    </row>
+    <row r="119" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C119" s="4"/>
+    </row>
+    <row r="120" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C120" s="4"/>
+    </row>
+    <row r="121" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C121" s="4"/>
+    </row>
+    <row r="122" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C122" s="4"/>
+    </row>
+    <row r="123" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C123" s="4"/>
+    </row>
+    <row r="124" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C124" s="4"/>
+    </row>
+    <row r="125" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C125" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G9" r:id="rId1" xr:uid="{B8E96A60-9B38-9D40-9947-E74D4A47B7D9}"/>
     <hyperlink ref="C7" r:id="rId2" xr:uid="{F4383ED6-1200-BB4F-80E8-DAD43B6E4946}"/>
     <hyperlink ref="G7" r:id="rId3" xr:uid="{EC8665CB-F279-D846-A7CF-82110EFEED8C}"/>
+    <hyperlink ref="G11:G15" r:id="rId4" display="https://git.generalassemb.ly/jdr-0622/sequelize-intro" xr:uid="{B69A30FC-A041-8243-8A0C-50F42F713089}"/>
+    <hyperlink ref="G29" r:id="rId5" xr:uid="{ABA8700E-0CD3-B748-B3DC-647F717D4F03}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1884,38 +2733,38 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
-        <v>150</v>
-      </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
+      <c r="A2" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
     </row>
     <row r="3" spans="1:8" s="11" customFormat="1" ht="38" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="H3" s="15" t="s">
         <v>25</v>
@@ -1923,210 +2772,210 @@
     </row>
     <row r="4" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E5" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="F5" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="F5" s="10" t="s">
-        <v>140</v>
-      </c>
       <c r="G5" s="10" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="61" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="57" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="G9" s="19" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="G10" s="18" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="18" x14ac:dyDescent="0.2">
@@ -2150,38 +2999,38 @@
       <c r="H13" s="10"/>
     </row>
     <row r="14" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="25" t="s">
-        <v>158</v>
-      </c>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
+      <c r="A14" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
     </row>
     <row r="15" spans="1:8" ht="38" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="H15" s="15" t="s">
         <v>25</v>
@@ -2189,184 +3038,184 @@
     </row>
     <row r="16" spans="1:8" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="G16" s="20" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="G17" s="20" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="H17" s="17" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
     </row>
     <row r="18" spans="1:8" s="21" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="G18" s="20" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="H18" s="17" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="D19" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="F19" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="G19" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="E19" s="17" t="s">
-        <v>163</v>
-      </c>
-      <c r="F19" s="20" t="s">
-        <v>169</v>
-      </c>
-      <c r="G19" s="20" t="s">
-        <v>170</v>
-      </c>
       <c r="H19" s="17" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="60" x14ac:dyDescent="0.2">
       <c r="A20" s="17" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="F20" s="20" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="G20" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="H20" s="17" t="s">
         <v>165</v>
-      </c>
-      <c r="H20" s="17" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A21" s="17" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="F21" s="20" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="G21" s="20" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="H21" s="17" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="F22" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="G22" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="H22" s="17" t="s">
         <v>169</v>
-      </c>
-      <c r="G22" s="20" t="s">
-        <v>177</v>
-      </c>
-      <c r="H22" s="17" t="s">
-        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -2379,11 +3228,868 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1D32C7E-648B-164D-A545-9CFFB679C2C8}">
+  <dimension ref="A1:H43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="48.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
+        <v>171</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="29" t="s">
+        <v>173</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>175</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>183</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>176</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>177</v>
+      </c>
+      <c r="G2" s="30" t="s">
+        <v>178</v>
+      </c>
+      <c r="H2" s="31" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="26" t="s">
+        <v>197</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="C3" s="25"/>
+      <c r="D3" s="36" t="s">
+        <v>181</v>
+      </c>
+      <c r="E3" s="36" t="s">
+        <v>180</v>
+      </c>
+      <c r="F3" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="G3" s="36" t="s">
+        <v>180</v>
+      </c>
+      <c r="H3" s="27"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="26" t="s">
+        <v>233</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="25"/>
+      <c r="D4" s="36" t="s">
+        <v>181</v>
+      </c>
+      <c r="E4" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="G4" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="H4" s="27" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="26" t="s">
+        <v>198</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="C5" s="25">
+        <v>255</v>
+      </c>
+      <c r="D5" s="36" t="s">
+        <v>181</v>
+      </c>
+      <c r="E5" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="F5" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="G5" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="H5" s="27" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="26" t="s">
+        <v>234</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="C6" s="25"/>
+      <c r="D6" s="36" t="s">
+        <v>181</v>
+      </c>
+      <c r="E6" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="F6" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="G6" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="H6" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="C7" s="25">
+        <v>255</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="E7" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="F7" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="G7" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="H7" s="27"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="26" t="s">
+        <v>236</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="C8" s="25"/>
+      <c r="D8" s="36" t="s">
+        <v>181</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="F8" s="36" t="s">
+        <v>180</v>
+      </c>
+      <c r="G8" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="H8" s="27"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="C9" s="25"/>
+      <c r="D9" s="36" t="s">
+        <v>181</v>
+      </c>
+      <c r="E9" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="F9" s="36" t="s">
+        <v>180</v>
+      </c>
+      <c r="G9" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="H9" s="27"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="C10" s="25"/>
+      <c r="D10" s="36" t="s">
+        <v>181</v>
+      </c>
+      <c r="E10" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="F10" s="36" t="s">
+        <v>180</v>
+      </c>
+      <c r="G10" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="H10" s="27"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="26" t="s">
+        <v>252</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="C11" s="25"/>
+      <c r="D11" s="36" t="s">
+        <v>181</v>
+      </c>
+      <c r="E11" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="F11" s="36" t="s">
+        <v>180</v>
+      </c>
+      <c r="G11" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="H11" s="27"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="C12" s="25"/>
+      <c r="D12" s="36" t="s">
+        <v>181</v>
+      </c>
+      <c r="E12" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="F12" s="36" t="s">
+        <v>180</v>
+      </c>
+      <c r="G12" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="H12" s="27"/>
+    </row>
+    <row r="15" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="A15" s="28" t="s">
+        <v>171</v>
+      </c>
+      <c r="B15" s="28" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="29" t="s">
+        <v>173</v>
+      </c>
+      <c r="B16" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="C16" s="30" t="s">
+        <v>175</v>
+      </c>
+      <c r="D16" s="30" t="s">
+        <v>183</v>
+      </c>
+      <c r="E16" s="30" t="s">
+        <v>176</v>
+      </c>
+      <c r="F16" s="30" t="s">
+        <v>177</v>
+      </c>
+      <c r="G16" s="30" t="s">
+        <v>178</v>
+      </c>
+      <c r="H16" s="31" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="26" t="s">
+        <v>197</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="C17" s="25"/>
+      <c r="D17" s="36" t="s">
+        <v>181</v>
+      </c>
+      <c r="E17" s="36" t="s">
+        <v>180</v>
+      </c>
+      <c r="F17" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="G17" s="36" t="s">
+        <v>180</v>
+      </c>
+      <c r="H17" s="27"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="26" t="s">
+        <v>198</v>
+      </c>
+      <c r="B18" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="C18" s="25">
+        <v>255</v>
+      </c>
+      <c r="D18" s="36" t="s">
+        <v>181</v>
+      </c>
+      <c r="E18" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="F18" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="G18" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="H18" s="27" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="26" t="s">
+        <v>219</v>
+      </c>
+      <c r="B19" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="C19" s="25"/>
+      <c r="D19" s="36" t="s">
+        <v>181</v>
+      </c>
+      <c r="E19" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="F19" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="G19" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="H19" s="27" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="26" t="s">
+        <v>220</v>
+      </c>
+      <c r="B20" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="C20" s="25"/>
+      <c r="D20" s="36" t="s">
+        <v>181</v>
+      </c>
+      <c r="E20" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="F20" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="G20" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="H20" s="27" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="A22" s="28" t="s">
+        <v>171</v>
+      </c>
+      <c r="B22" s="28" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="29" t="s">
+        <v>173</v>
+      </c>
+      <c r="B23" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="C23" s="30" t="s">
+        <v>175</v>
+      </c>
+      <c r="D23" s="30" t="s">
+        <v>183</v>
+      </c>
+      <c r="E23" s="30" t="s">
+        <v>176</v>
+      </c>
+      <c r="F23" s="30" t="s">
+        <v>177</v>
+      </c>
+      <c r="G23" s="30" t="s">
+        <v>178</v>
+      </c>
+      <c r="H23" s="31" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="26" t="s">
+        <v>197</v>
+      </c>
+      <c r="B24" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="C24" s="25"/>
+      <c r="D24" s="36" t="s">
+        <v>181</v>
+      </c>
+      <c r="E24" s="36" t="s">
+        <v>180</v>
+      </c>
+      <c r="F24" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="G24" s="36" t="s">
+        <v>180</v>
+      </c>
+      <c r="H24" s="27"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="26" t="s">
+        <v>198</v>
+      </c>
+      <c r="B25" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="C25" s="25">
+        <v>255</v>
+      </c>
+      <c r="D25" s="36" t="s">
+        <v>181</v>
+      </c>
+      <c r="E25" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="F25" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="G25" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="H25" s="27" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="26" t="s">
+        <v>219</v>
+      </c>
+      <c r="B26" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="C26" s="25"/>
+      <c r="D26" s="36" t="s">
+        <v>181</v>
+      </c>
+      <c r="E26" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="F26" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="G26" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="H26" s="27" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="26" t="s">
+        <v>220</v>
+      </c>
+      <c r="B27" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="C27" s="25"/>
+      <c r="D27" s="36" t="s">
+        <v>181</v>
+      </c>
+      <c r="E27" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="F27" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="G27" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="H27" s="27" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="A29" s="28" t="s">
+        <v>171</v>
+      </c>
+      <c r="B29" s="28" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="29" t="s">
+        <v>173</v>
+      </c>
+      <c r="B30" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="C30" s="30" t="s">
+        <v>175</v>
+      </c>
+      <c r="D30" s="30" t="s">
+        <v>183</v>
+      </c>
+      <c r="E30" s="30" t="s">
+        <v>176</v>
+      </c>
+      <c r="F30" s="30" t="s">
+        <v>177</v>
+      </c>
+      <c r="G30" s="30" t="s">
+        <v>178</v>
+      </c>
+      <c r="H30" s="31" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="26" t="s">
+        <v>197</v>
+      </c>
+      <c r="B31" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="C31" s="25"/>
+      <c r="D31" s="36" t="s">
+        <v>181</v>
+      </c>
+      <c r="E31" s="36" t="s">
+        <v>180</v>
+      </c>
+      <c r="F31" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="G31" s="36" t="s">
+        <v>180</v>
+      </c>
+      <c r="H31" s="27"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="26" t="s">
+        <v>198</v>
+      </c>
+      <c r="B32" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="C32" s="25">
+        <v>255</v>
+      </c>
+      <c r="D32" s="36" t="s">
+        <v>181</v>
+      </c>
+      <c r="E32" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="F32" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="G32" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="H32" s="27" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="26" t="s">
+        <v>219</v>
+      </c>
+      <c r="B33" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="C33" s="25"/>
+      <c r="D33" s="36" t="s">
+        <v>181</v>
+      </c>
+      <c r="E33" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="F33" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="G33" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="H33" s="27" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="26" t="s">
+        <v>220</v>
+      </c>
+      <c r="B34" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="C34" s="25"/>
+      <c r="D34" s="36" t="s">
+        <v>181</v>
+      </c>
+      <c r="E34" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="F34" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="G34" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="H34" s="27" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="A36" s="28" t="s">
+        <v>171</v>
+      </c>
+      <c r="B36" s="28" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="29" t="s">
+        <v>173</v>
+      </c>
+      <c r="B37" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="C37" s="30" t="s">
+        <v>175</v>
+      </c>
+      <c r="D37" s="30" t="s">
+        <v>183</v>
+      </c>
+      <c r="E37" s="30" t="s">
+        <v>176</v>
+      </c>
+      <c r="F37" s="30" t="s">
+        <v>177</v>
+      </c>
+      <c r="G37" s="30" t="s">
+        <v>178</v>
+      </c>
+      <c r="H37" s="31" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="26" t="s">
+        <v>197</v>
+      </c>
+      <c r="B38" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="C38" s="25"/>
+      <c r="D38" s="36" t="s">
+        <v>181</v>
+      </c>
+      <c r="E38" s="36" t="s">
+        <v>180</v>
+      </c>
+      <c r="F38" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="G38" s="36" t="s">
+        <v>180</v>
+      </c>
+      <c r="H38" s="27"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="26" t="s">
+        <v>198</v>
+      </c>
+      <c r="B39" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="C39" s="25">
+        <v>255</v>
+      </c>
+      <c r="D39" s="36" t="s">
+        <v>181</v>
+      </c>
+      <c r="E39" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="F39" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="G39" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="H39" s="27" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="26" t="s">
+        <v>249</v>
+      </c>
+      <c r="B40" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="C40" s="25">
+        <v>255</v>
+      </c>
+      <c r="D40" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="E40" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="F40" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="G40" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="H40" s="27"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="26" t="s">
+        <v>250</v>
+      </c>
+      <c r="B41" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="C41" s="25">
+        <v>255</v>
+      </c>
+      <c r="D41" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="E41" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="F41" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="G41" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="H41" s="27"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" s="26" t="s">
+        <v>219</v>
+      </c>
+      <c r="B42" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="C42" s="25"/>
+      <c r="D42" s="36" t="s">
+        <v>181</v>
+      </c>
+      <c r="E42" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="F42" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="G42" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="H42" s="27" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" s="26" t="s">
+        <v>220</v>
+      </c>
+      <c r="B43" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="C43" s="25"/>
+      <c r="D43" s="36" t="s">
+        <v>181</v>
+      </c>
+      <c r="E43" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="F43" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="G43" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="H43" s="27" t="s">
+        <v>190</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFD95FFD-3F78-284D-BA72-713E3F9CEBC1}">
   <dimension ref="A2:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Commit: All tables loaded with seeders
</commit_message>
<xml_diff>
--- a/documentation/Expense_Tracker_App_plan.xlsx
+++ b/documentation/Expense_Tracker_App_plan.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ct08284/sei/projects/deere-project2-starter/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D58AF90B-4939-1442-962F-4E037B22D3D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77B638A-8D41-524B-9B9C-E5E7C4B52AAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" xr2:uid="{05595CE3-5133-A840-8AB2-952878BB912B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" activeTab="4" xr2:uid="{05595CE3-5133-A840-8AB2-952878BB912B}"/>
   </bookViews>
   <sheets>
     <sheet name="Development_plan" sheetId="2" r:id="rId1"/>
     <sheet name="MVP features" sheetId="1" r:id="rId2"/>
     <sheet name="RESTFUL routing" sheetId="5" r:id="rId3"/>
     <sheet name="Table definitions" sheetId="6" r:id="rId4"/>
-    <sheet name="Resources" sheetId="3" r:id="rId5"/>
+    <sheet name="Default Values" sheetId="8" r:id="rId5"/>
+    <sheet name="Resources" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="299">
   <si>
     <t>Feature #</t>
   </si>
@@ -820,6 +821,141 @@
   </si>
   <si>
     <t>statusId</t>
+  </si>
+  <si>
+    <t>seeders/timestamp-demo-subaccounts.js</t>
+  </si>
+  <si>
+    <t>Family</t>
+  </si>
+  <si>
+    <t>Father</t>
+  </si>
+  <si>
+    <t>Mother</t>
+  </si>
+  <si>
+    <t>Son</t>
+  </si>
+  <si>
+    <t>Daughter</t>
+  </si>
+  <si>
+    <t>Education</t>
+  </si>
+  <si>
+    <t>Enterteinment</t>
+  </si>
+  <si>
+    <t>Food</t>
+  </si>
+  <si>
+    <t>Vacations</t>
+  </si>
+  <si>
+    <t>Clothing</t>
+  </si>
+  <si>
+    <t>Health care</t>
+  </si>
+  <si>
+    <t>Transportation</t>
+  </si>
+  <si>
+    <t>Other necessities</t>
+  </si>
+  <si>
+    <t>Cash</t>
+  </si>
+  <si>
+    <t>Credit card</t>
+  </si>
+  <si>
+    <t>Bank transfer</t>
+  </si>
+  <si>
+    <t>Prepaid card</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>#FFFFFF</t>
+  </si>
+  <si>
+    <t>BackgroundColor</t>
+  </si>
+  <si>
+    <t>#FF2600</t>
+  </si>
+  <si>
+    <t>#000000</t>
+  </si>
+  <si>
+    <t>#F4F4F4</t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>"2020-07-31"</t>
+  </si>
+  <si>
+    <t>Restaurant Meal</t>
+  </si>
+  <si>
+    <t>Cinema</t>
+  </si>
+  <si>
+    <t>Dentist</t>
+  </si>
+  <si>
+    <t>Taxes</t>
+  </si>
+  <si>
+    <t>Car Wash</t>
+  </si>
+  <si>
+    <t>Tennis shoes</t>
+  </si>
+  <si>
+    <t>New laptop</t>
+  </si>
+  <si>
+    <t>New smartphone</t>
+  </si>
+  <si>
+    <t>Flight tickets</t>
+  </si>
+  <si>
+    <t>Suitcases</t>
+  </si>
+  <si>
+    <t>"2020-07-15"</t>
+  </si>
+  <si>
+    <t>"2020-07-16"</t>
+  </si>
+  <si>
+    <t>"2020-07-20"</t>
+  </si>
+  <si>
+    <t>"2020-08-01"</t>
+  </si>
+  <si>
+    <t>"2020-08-02"</t>
+  </si>
+  <si>
+    <t>Red Lobster</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>American Airlines</t>
   </si>
 </sst>
 </file>
@@ -1017,7 +1153,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1093,6 +1229,7 @@
     </xf>
     <xf numFmtId="15" fontId="1" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1116,6 +1253,7 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1433,8 +1571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FFC9C39-9695-8A40-8D81-C0586B568F96}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23:F31"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1736,7 +1874,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="39">
+      <c r="A16" s="40">
         <v>10</v>
       </c>
       <c r="B16" s="33" t="s">
@@ -1747,13 +1885,13 @@
       <c r="E16" s="35">
         <v>44045</v>
       </c>
-      <c r="F16" s="38" t="s">
+      <c r="F16" s="39" t="s">
         <v>88</v>
       </c>
       <c r="G16" s="5"/>
     </row>
     <row r="17" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="37">
+      <c r="A17" s="38">
         <v>10.1</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1816,7 +1954,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="37">
+      <c r="A20" s="38">
         <v>10.199999999999999</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -1879,7 +2017,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="37">
+      <c r="A23" s="38">
         <v>10.3</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -1942,7 +2080,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="37">
+      <c r="A26" s="38">
         <v>10.4</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -2005,7 +2143,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="37">
+      <c r="A29" s="38">
         <v>10.5</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -2068,7 +2206,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="39">
+      <c r="A32" s="40">
         <v>11</v>
       </c>
       <c r="B32" s="33" t="s">
@@ -2079,7 +2217,7 @@
       <c r="E32" s="35">
         <v>44045</v>
       </c>
-      <c r="F32" s="45" t="s">
+      <c r="F32" s="46" t="s">
         <v>87</v>
       </c>
       <c r="G32" s="5" t="s">
@@ -2087,128 +2225,140 @@
       </c>
     </row>
     <row r="33" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A33" s="40">
+      <c r="A33" s="41">
         <v>11.1</v>
       </c>
       <c r="B33" s="21" t="s">
         <v>239</v>
       </c>
-      <c r="C33" s="41" t="s">
+      <c r="C33" s="42" t="s">
         <v>244</v>
       </c>
-      <c r="D33" s="41" t="s">
+      <c r="D33" s="42" t="s">
         <v>248</v>
       </c>
-      <c r="E33" s="42"/>
-      <c r="F33" s="45" t="s">
-        <v>87</v>
-      </c>
-      <c r="G33" s="44"/>
+      <c r="E33" s="43"/>
+      <c r="F33" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="34" spans="1:7" ht="68" x14ac:dyDescent="0.2">
-      <c r="A34" s="40">
+      <c r="A34" s="41">
         <v>11.11</v>
       </c>
       <c r="B34" s="21" t="s">
         <v>241</v>
       </c>
-      <c r="C34" s="41" t="s">
+      <c r="C34" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="D34" s="41"/>
-      <c r="E34" s="42"/>
-      <c r="F34" s="43"/>
-      <c r="G34" s="44"/>
+      <c r="D34" s="42"/>
+      <c r="E34" s="43"/>
+      <c r="F34" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="35" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A35" s="40">
+      <c r="A35" s="41">
         <v>11.2</v>
       </c>
       <c r="B35" s="21" t="s">
         <v>240</v>
       </c>
-      <c r="C35" s="41" t="s">
+      <c r="C35" s="42" t="s">
         <v>245</v>
       </c>
-      <c r="D35" s="41"/>
-      <c r="E35" s="42"/>
-      <c r="F35" s="43"/>
-      <c r="G35" s="44"/>
+      <c r="D35" s="42" t="s">
+        <v>254</v>
+      </c>
+      <c r="E35" s="43"/>
+      <c r="F35" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="G35" s="45"/>
     </row>
     <row r="36" spans="1:7" ht="68" x14ac:dyDescent="0.2">
-      <c r="A36" s="40">
+      <c r="A36" s="41">
         <v>11.21</v>
       </c>
       <c r="B36" s="21" t="s">
         <v>241</v>
       </c>
-      <c r="C36" s="41" t="s">
+      <c r="C36" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="D36" s="41"/>
-      <c r="E36" s="42"/>
-      <c r="F36" s="43"/>
-      <c r="G36" s="44"/>
+      <c r="D36" s="42"/>
+      <c r="E36" s="43"/>
+      <c r="F36" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="G36" s="45"/>
     </row>
     <row r="37" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" s="40">
+      <c r="A37" s="41">
         <v>11.3</v>
       </c>
       <c r="B37" s="21" t="s">
         <v>242</v>
       </c>
-      <c r="C37" s="41" t="s">
+      <c r="C37" s="42" t="s">
         <v>246</v>
       </c>
-      <c r="D37" s="41"/>
-      <c r="E37" s="42"/>
-      <c r="F37" s="43"/>
-      <c r="G37" s="44"/>
+      <c r="D37" s="42"/>
+      <c r="E37" s="43"/>
+      <c r="F37" s="44"/>
+      <c r="G37" s="45"/>
     </row>
     <row r="38" spans="1:7" ht="68" x14ac:dyDescent="0.2">
-      <c r="A38" s="40">
+      <c r="A38" s="41">
         <v>11.31</v>
       </c>
       <c r="B38" s="21" t="s">
         <v>241</v>
       </c>
-      <c r="C38" s="41" t="s">
+      <c r="C38" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="D38" s="41"/>
-      <c r="E38" s="42"/>
-      <c r="F38" s="43"/>
-      <c r="G38" s="44"/>
+      <c r="D38" s="42"/>
+      <c r="E38" s="43"/>
+      <c r="F38" s="44"/>
+      <c r="G38" s="45"/>
     </row>
     <row r="39" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A39" s="40">
+      <c r="A39" s="41">
         <v>11.4</v>
       </c>
       <c r="B39" s="21" t="s">
         <v>243</v>
       </c>
-      <c r="C39" s="41" t="s">
+      <c r="C39" s="42" t="s">
         <v>247</v>
       </c>
-      <c r="D39" s="41"/>
-      <c r="E39" s="42"/>
-      <c r="F39" s="43"/>
-      <c r="G39" s="44"/>
+      <c r="D39" s="42"/>
+      <c r="E39" s="43"/>
+      <c r="F39" s="44"/>
+      <c r="G39" s="45"/>
     </row>
     <row r="40" spans="1:7" ht="68" x14ac:dyDescent="0.2">
-      <c r="A40" s="40">
+      <c r="A40" s="41">
         <v>11.41</v>
       </c>
       <c r="B40" s="21" t="s">
         <v>241</v>
       </c>
-      <c r="C40" s="41" t="s">
+      <c r="C40" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="D40" s="41"/>
-      <c r="E40" s="42"/>
-      <c r="F40" s="43"/>
-      <c r="G40" s="44"/>
+      <c r="D40" s="42"/>
+      <c r="E40" s="43"/>
+      <c r="F40" s="44"/>
+      <c r="G40" s="45"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="7">
@@ -4085,6 +4235,623 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{548A6984-5372-3942-B42C-A3C7DE1E5AD2}">
+  <dimension ref="A2:J45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
+        <v>171</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="26">
+        <v>1</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="26">
+        <v>2</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="26">
+        <v>3</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="26">
+        <v>4</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="26">
+        <v>5</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="A10" s="28" t="s">
+        <v>171</v>
+      </c>
+      <c r="B10" s="28" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="B11" s="30" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="26">
+        <v>1</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="26">
+        <v>2</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="26">
+        <v>3</v>
+      </c>
+      <c r="B14" s="25" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="26">
+        <v>4</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="26">
+        <v>5</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="26">
+        <v>6</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="26">
+        <v>7</v>
+      </c>
+      <c r="B18" s="25" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="26">
+        <v>8</v>
+      </c>
+      <c r="B19" s="25" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="37"/>
+      <c r="B20" s="37"/>
+    </row>
+    <row r="21" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A21" s="28" t="s">
+        <v>171</v>
+      </c>
+      <c r="B21" s="28" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="B22" s="30" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="26">
+        <v>1</v>
+      </c>
+      <c r="B23" s="25" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="26">
+        <v>2</v>
+      </c>
+      <c r="B24" s="25" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="26">
+        <v>3</v>
+      </c>
+      <c r="B25" s="25" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="26">
+        <v>4</v>
+      </c>
+      <c r="B26" s="25" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="26">
+        <v>5</v>
+      </c>
+      <c r="B27" s="25" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="37"/>
+      <c r="B28" s="37"/>
+    </row>
+    <row r="29" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A29" s="28" t="s">
+        <v>171</v>
+      </c>
+      <c r="B29" s="28" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="B30" s="30" t="s">
+        <v>198</v>
+      </c>
+      <c r="C30" s="30" t="s">
+        <v>249</v>
+      </c>
+      <c r="D30" s="30" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="26">
+        <v>1</v>
+      </c>
+      <c r="B31" s="25" t="s">
+        <v>279</v>
+      </c>
+      <c r="C31" s="25" t="s">
+        <v>277</v>
+      </c>
+      <c r="D31" s="25" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="26">
+        <v>2</v>
+      </c>
+      <c r="B32" s="25" t="s">
+        <v>273</v>
+      </c>
+      <c r="C32" s="25" t="s">
+        <v>274</v>
+      </c>
+      <c r="D32" s="25" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+      <c r="A34" s="28" t="s">
+        <v>171</v>
+      </c>
+      <c r="B34" s="28" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="B35" s="30" t="s">
+        <v>233</v>
+      </c>
+      <c r="C35" s="30" t="s">
+        <v>198</v>
+      </c>
+      <c r="D35" s="30" t="s">
+        <v>234</v>
+      </c>
+      <c r="E35" s="30" t="s">
+        <v>235</v>
+      </c>
+      <c r="F35" s="30" t="s">
+        <v>236</v>
+      </c>
+      <c r="G35" s="30" t="s">
+        <v>172</v>
+      </c>
+      <c r="H35" s="30" t="s">
+        <v>251</v>
+      </c>
+      <c r="I35" s="30" t="s">
+        <v>252</v>
+      </c>
+      <c r="J35" s="30" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>1</v>
+      </c>
+      <c r="B36" s="47" t="s">
+        <v>291</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D36" s="38">
+        <v>120</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="F36" s="1">
+        <v>1</v>
+      </c>
+      <c r="G36" s="1">
+        <v>1</v>
+      </c>
+      <c r="H36" s="1">
+        <v>2</v>
+      </c>
+      <c r="I36" s="1">
+        <v>2</v>
+      </c>
+      <c r="J36" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>2</v>
+      </c>
+      <c r="B37" s="47" t="s">
+        <v>292</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="D37" s="38">
+        <v>20</v>
+      </c>
+      <c r="F37" s="1">
+        <v>1</v>
+      </c>
+      <c r="G37" s="1">
+        <v>3</v>
+      </c>
+      <c r="H37" s="1">
+        <v>2</v>
+      </c>
+      <c r="I37" s="1">
+        <v>1</v>
+      </c>
+      <c r="J37" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>3</v>
+      </c>
+      <c r="B38" s="47" t="s">
+        <v>292</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="D38" s="38">
+        <v>40</v>
+      </c>
+      <c r="F38" s="1">
+        <v>1</v>
+      </c>
+      <c r="G38" s="1">
+        <v>2</v>
+      </c>
+      <c r="H38" s="1">
+        <v>6</v>
+      </c>
+      <c r="I38" s="1">
+        <v>2</v>
+      </c>
+      <c r="J38" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>4</v>
+      </c>
+      <c r="B39" s="47" t="s">
+        <v>293</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="D39" s="38">
+        <v>150</v>
+      </c>
+      <c r="F39" s="1">
+        <v>1</v>
+      </c>
+      <c r="G39" s="1">
+        <v>1</v>
+      </c>
+      <c r="H39" s="1">
+        <v>8</v>
+      </c>
+      <c r="I39" s="1">
+        <v>3</v>
+      </c>
+      <c r="J39" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>5</v>
+      </c>
+      <c r="B40" s="47" t="s">
+        <v>293</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D40" s="38">
+        <v>20</v>
+      </c>
+      <c r="F40" s="1">
+        <v>1</v>
+      </c>
+      <c r="G40" s="1">
+        <v>3</v>
+      </c>
+      <c r="H40" s="1">
+        <v>8</v>
+      </c>
+      <c r="I40" s="1">
+        <v>1</v>
+      </c>
+      <c r="J40" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <v>6</v>
+      </c>
+      <c r="B41" s="47" t="s">
+        <v>293</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D41" s="38">
+        <v>80</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="F41" s="1">
+        <v>1</v>
+      </c>
+      <c r="G41" s="1">
+        <v>2</v>
+      </c>
+      <c r="H41" s="1">
+        <v>5</v>
+      </c>
+      <c r="I41" s="1">
+        <v>4</v>
+      </c>
+      <c r="J41" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <v>7</v>
+      </c>
+      <c r="B42" s="47" t="s">
+        <v>280</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="D42" s="38">
+        <v>500</v>
+      </c>
+      <c r="F42" s="1">
+        <v>1</v>
+      </c>
+      <c r="G42" s="1">
+        <v>4</v>
+      </c>
+      <c r="H42" s="1">
+        <v>1</v>
+      </c>
+      <c r="I42" s="1">
+        <v>2</v>
+      </c>
+      <c r="J42" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <v>8</v>
+      </c>
+      <c r="B43" s="47" t="s">
+        <v>294</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D43" s="38">
+        <v>300</v>
+      </c>
+      <c r="F43" s="1">
+        <v>1</v>
+      </c>
+      <c r="G43" s="1">
+        <v>3</v>
+      </c>
+      <c r="H43" s="1">
+        <v>8</v>
+      </c>
+      <c r="I43" s="1">
+        <v>2</v>
+      </c>
+      <c r="J43" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <v>9</v>
+      </c>
+      <c r="B44" s="47" t="s">
+        <v>294</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="D44" s="38">
+        <v>800</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="F44" s="1">
+        <v>1</v>
+      </c>
+      <c r="G44" s="1">
+        <v>1</v>
+      </c>
+      <c r="H44" s="1">
+        <v>4</v>
+      </c>
+      <c r="I44" s="1">
+        <v>2</v>
+      </c>
+      <c r="J44" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <v>10</v>
+      </c>
+      <c r="B45" s="47" t="s">
+        <v>295</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="D45" s="38">
+        <v>120</v>
+      </c>
+      <c r="F45" s="1">
+        <v>1</v>
+      </c>
+      <c r="G45" s="1">
+        <v>1</v>
+      </c>
+      <c r="H45" s="1">
+        <v>4</v>
+      </c>
+      <c r="I45" s="1">
+        <v>2</v>
+      </c>
+      <c r="J45" s="1">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFD95FFD-3F78-284D-BA72-713E3F9CEBC1}">
   <dimension ref="A2:B24"/>
   <sheetViews>

</xml_diff>

<commit_message>
Route:Index Functions: Filtering Status: Account and Subaccount complete
</commit_message>
<xml_diff>
--- a/documentation/Expense_Tracker_App_plan.xlsx
+++ b/documentation/Expense_Tracker_App_plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ct08284/sei/projects/deere-project2-starter/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77B638A-8D41-524B-9B9C-E5E7C4B52AAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA0332CE-FD68-2B4B-9E38-3BAE4A629BD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" activeTab="4" xr2:uid="{05595CE3-5133-A840-8AB2-952878BB912B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" xr2:uid="{05595CE3-5133-A840-8AB2-952878BB912B}"/>
   </bookViews>
   <sheets>
     <sheet name="Development_plan" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="309">
   <si>
     <t>Feature #</t>
   </si>
@@ -278,11 +278,6 @@
   </si>
   <si>
     <t>Resources</t>
-  </si>
-  <si>
-    <t>(1) sequelize db:seed:all
- OR
-(2) sequelize db:seed --seed seeders/20200726194746-demo-users.js</t>
   </si>
   <si>
     <t>Excel</t>
@@ -956,6 +951,49 @@
   </si>
   <si>
     <t>American Airlines</t>
+  </si>
+  <si>
+    <t>Best Buy</t>
+  </si>
+  <si>
+    <t>Create seeder for Expenses table</t>
+  </si>
+  <si>
+    <t>npx sequelize seed:generate --name demo-expenses</t>
+  </si>
+  <si>
+    <t>(1) sequelize db:seed:all
+ OR
+(2) sequelize db:seed --seed seeders/timestamp-demo-expenses.js</t>
+  </si>
+  <si>
+    <t>(1) sequelize db:seed:all
+ OR
+(2) sequelize db:seed --seed seeders/timestamp-demo-statuses.js</t>
+  </si>
+  <si>
+    <t>(1) sequelize db:seed:all
+ OR
+(2) sequelize db:seed --seed seeders/timestamp-demo-paymentTypes.js</t>
+  </si>
+  <si>
+    <t>(1) sequelize db:seed:all
+ OR
+(2) sequelize db:seed --seed seeders/timestamp-demo-subaccounts.js</t>
+  </si>
+  <si>
+    <t>(1) sequelize db:seed:all
+ OR
+(2) sequelize db:seed --seed seeders/timestamp-demo-accounts.js</t>
+  </si>
+  <si>
+    <t>seeders/timestamp-demo-paymentTypes.js</t>
+  </si>
+  <si>
+    <t>seeders/timestamp-demo-statuses.js</t>
+  </si>
+  <si>
+    <t>seeders/timestamp-demo-expenses.js</t>
   </si>
 </sst>
 </file>
@@ -1153,7 +1191,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1201,12 +1239,6 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1244,9 +1276,6 @@
     <xf numFmtId="15" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1254,6 +1283,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1569,10 +1604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FFC9C39-9695-8A40-8D81-C0586B568F96}">
-  <dimension ref="A1:G125"/>
+  <dimension ref="A1:G127"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1622,7 +1657,7 @@
         <v>44043</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -1637,7 +1672,7 @@
         <v>44043</v>
       </c>
       <c r="F3" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -1652,10 +1687,10 @@
         <v>44044</v>
       </c>
       <c r="F4" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -1670,10 +1705,10 @@
         <v>44044</v>
       </c>
       <c r="F5" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1684,13 +1719,13 @@
         <v>70</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E6" s="6">
         <v>44044</v>
       </c>
-      <c r="F6" s="32" t="s">
-        <v>87</v>
+      <c r="F6" s="30" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -1698,22 +1733,22 @@
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="D7" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="E7" s="6">
         <v>44045</v>
       </c>
       <c r="F7" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1733,7 +1768,7 @@
         <v>44045</v>
       </c>
       <c r="F8" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1753,26 +1788,26 @@
         <v>44045</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="33">
+      <c r="A10" s="31">
         <v>9</v>
       </c>
-      <c r="B10" s="33" t="s">
+      <c r="B10" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="35">
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="33">
         <v>44045</v>
       </c>
       <c r="F10" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G10" s="5"/>
     </row>
@@ -1781,17 +1816,17 @@
         <v>9.1</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>192</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>193</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>31</v>
@@ -1802,15 +1837,15 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>31</v>
@@ -1821,15 +1856,15 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>31</v>
@@ -1840,15 +1875,15 @@
         <v>9.4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>31</v>
@@ -1859,53 +1894,53 @@
         <v>9.5</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="40">
+      <c r="A16" s="38">
         <v>10</v>
       </c>
-      <c r="B16" s="33" t="s">
-        <v>215</v>
-      </c>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="35">
+      <c r="B16" s="31" t="s">
+        <v>214</v>
+      </c>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="33">
         <v>44045</v>
       </c>
-      <c r="F16" s="39" t="s">
-        <v>88</v>
+      <c r="F16" s="37" t="s">
+        <v>87</v>
       </c>
       <c r="G16" s="5"/>
     </row>
     <row r="17" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="38">
+      <c r="A17" s="36">
         <v>10.1</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>75</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>31</v>
@@ -1916,17 +1951,17 @@
         <v>10.11</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>75</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>31</v>
@@ -1937,38 +1972,38 @@
         <v>10.119999999999999</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>78</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="38">
+      <c r="A20" s="36">
         <v>10.199999999999999</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>75</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>31</v>
@@ -1979,17 +2014,17 @@
         <v>10.210000000000001</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>75</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E21" s="6"/>
       <c r="F21" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>31</v>
@@ -2000,38 +2035,38 @@
         <v>10.220000000000001</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>78</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E22" s="6"/>
       <c r="F22" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="38">
+      <c r="A23" s="36">
         <v>10.3</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>75</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E23" s="6"/>
       <c r="F23" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>31</v>
@@ -2042,17 +2077,17 @@
         <v>10.31</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>75</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E24" s="6"/>
       <c r="F24" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G24" s="5" t="s">
         <v>31</v>
@@ -2063,38 +2098,38 @@
         <v>10.32</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>78</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E25" s="6"/>
       <c r="F25" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="38">
+      <c r="A26" s="36">
         <v>10.4</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>75</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E26" s="6"/>
       <c r="F26" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G26" s="5" t="s">
         <v>31</v>
@@ -2105,17 +2140,17 @@
         <v>10.41</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>75</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E27" s="6"/>
       <c r="F27" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>31</v>
@@ -2126,41 +2161,41 @@
         <v>10.42</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>78</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E28" s="6"/>
       <c r="F28" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G28" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="38">
+      <c r="A29" s="36">
         <v>10.5</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>75</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -2168,17 +2203,17 @@
         <v>10.51</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>75</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E30" s="6"/>
       <c r="F30" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G30" s="5" t="s">
         <v>31</v>
@@ -2189,195 +2224,233 @@
         <v>10.52</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>78</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E31" s="6"/>
       <c r="F31" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G31" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="40">
+      <c r="A32" s="38">
         <v>11</v>
       </c>
-      <c r="B32" s="33" t="s">
-        <v>238</v>
-      </c>
-      <c r="C32" s="34"/>
-      <c r="D32" s="34"/>
-      <c r="E32" s="35">
+      <c r="B32" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="C32" s="32"/>
+      <c r="D32" s="32"/>
+      <c r="E32" s="33">
         <v>44045</v>
       </c>
-      <c r="F32" s="46" t="s">
-        <v>87</v>
+      <c r="F32" s="43" t="s">
+        <v>86</v>
       </c>
       <c r="G32" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A33" s="41">
+      <c r="A33" s="39">
         <v>11.1</v>
       </c>
       <c r="B33" s="21" t="s">
-        <v>239</v>
-      </c>
-      <c r="C33" s="42" t="s">
-        <v>244</v>
-      </c>
-      <c r="D33" s="42" t="s">
-        <v>248</v>
-      </c>
-      <c r="E33" s="43"/>
+        <v>238</v>
+      </c>
+      <c r="C33" s="40" t="s">
+        <v>243</v>
+      </c>
+      <c r="D33" s="40" t="s">
+        <v>247</v>
+      </c>
+      <c r="E33" s="41"/>
       <c r="F33" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G33" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="68" x14ac:dyDescent="0.2">
-      <c r="A34" s="41">
+      <c r="A34" s="39">
         <v>11.11</v>
       </c>
       <c r="B34" s="21" t="s">
-        <v>241</v>
-      </c>
-      <c r="C34" s="42" t="s">
-        <v>80</v>
-      </c>
-      <c r="D34" s="42"/>
-      <c r="E34" s="43"/>
+        <v>240</v>
+      </c>
+      <c r="C34" s="40" t="s">
+        <v>305</v>
+      </c>
+      <c r="D34" s="40"/>
+      <c r="E34" s="41"/>
       <c r="F34" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G34" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A35" s="41">
+      <c r="A35" s="39">
         <v>11.2</v>
       </c>
       <c r="B35" s="21" t="s">
+        <v>239</v>
+      </c>
+      <c r="C35" s="40" t="s">
+        <v>244</v>
+      </c>
+      <c r="D35" s="40" t="s">
+        <v>253</v>
+      </c>
+      <c r="E35" s="41"/>
+      <c r="F35" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="G35" s="42"/>
+    </row>
+    <row r="36" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A36" s="39">
+        <v>11.21</v>
+      </c>
+      <c r="B36" s="21" t="s">
         <v>240</v>
       </c>
-      <c r="C35" s="42" t="s">
+      <c r="C36" s="40" t="s">
+        <v>304</v>
+      </c>
+      <c r="D36" s="40"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="G36" s="42"/>
+    </row>
+    <row r="37" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" s="39">
+        <v>11.3</v>
+      </c>
+      <c r="B37" s="21" t="s">
+        <v>241</v>
+      </c>
+      <c r="C37" s="40" t="s">
         <v>245</v>
       </c>
-      <c r="D35" s="42" t="s">
-        <v>254</v>
-      </c>
-      <c r="E35" s="43"/>
-      <c r="F35" s="22" t="s">
-        <v>86</v>
-      </c>
-      <c r="G35" s="45"/>
-    </row>
-    <row r="36" spans="1:7" ht="68" x14ac:dyDescent="0.2">
-      <c r="A36" s="41">
-        <v>11.21</v>
-      </c>
-      <c r="B36" s="21" t="s">
-        <v>241</v>
-      </c>
-      <c r="C36" s="42" t="s">
-        <v>80</v>
-      </c>
-      <c r="D36" s="42"/>
-      <c r="E36" s="43"/>
-      <c r="F36" s="22" t="s">
-        <v>86</v>
-      </c>
-      <c r="G36" s="45"/>
-    </row>
-    <row r="37" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" s="41">
-        <v>11.3</v>
-      </c>
-      <c r="B37" s="21" t="s">
+      <c r="D37" s="40" t="s">
+        <v>306</v>
+      </c>
+      <c r="E37" s="41"/>
+      <c r="F37" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="G37" s="42"/>
+    </row>
+    <row r="38" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A38" s="39">
+        <v>11.31</v>
+      </c>
+      <c r="B38" s="21" t="s">
+        <v>240</v>
+      </c>
+      <c r="C38" s="40" t="s">
+        <v>303</v>
+      </c>
+      <c r="D38" s="40"/>
+      <c r="E38" s="41"/>
+      <c r="F38" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="G38" s="42"/>
+    </row>
+    <row r="39" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A39" s="39">
+        <v>11.4</v>
+      </c>
+      <c r="B39" s="21" t="s">
         <v>242</v>
       </c>
-      <c r="C37" s="42" t="s">
+      <c r="C39" s="40" t="s">
         <v>246</v>
       </c>
-      <c r="D37" s="42"/>
-      <c r="E37" s="43"/>
-      <c r="F37" s="44"/>
-      <c r="G37" s="45"/>
-    </row>
-    <row r="38" spans="1:7" ht="68" x14ac:dyDescent="0.2">
-      <c r="A38" s="41">
-        <v>11.31</v>
-      </c>
-      <c r="B38" s="21" t="s">
-        <v>241</v>
-      </c>
-      <c r="C38" s="42" t="s">
-        <v>80</v>
-      </c>
-      <c r="D38" s="42"/>
-      <c r="E38" s="43"/>
-      <c r="F38" s="44"/>
-      <c r="G38" s="45"/>
-    </row>
-    <row r="39" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A39" s="41">
-        <v>11.4</v>
-      </c>
-      <c r="B39" s="21" t="s">
-        <v>243</v>
-      </c>
-      <c r="C39" s="42" t="s">
-        <v>247</v>
-      </c>
-      <c r="D39" s="42"/>
-      <c r="E39" s="43"/>
-      <c r="F39" s="44"/>
-      <c r="G39" s="45"/>
+      <c r="D39" s="40" t="s">
+        <v>307</v>
+      </c>
+      <c r="E39" s="41"/>
+      <c r="F39" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="G39" s="42"/>
     </row>
     <row r="40" spans="1:7" ht="68" x14ac:dyDescent="0.2">
-      <c r="A40" s="41">
+      <c r="A40" s="39">
         <v>11.41</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>241</v>
-      </c>
-      <c r="C40" s="42" t="s">
-        <v>80</v>
-      </c>
-      <c r="D40" s="42"/>
-      <c r="E40" s="43"/>
-      <c r="F40" s="44"/>
-      <c r="G40" s="45"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="7">
+        <v>240</v>
+      </c>
+      <c r="C40" s="40" t="s">
+        <v>302</v>
+      </c>
+      <c r="D40" s="40"/>
+      <c r="E40" s="41"/>
+      <c r="F40" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="G40" s="42"/>
+    </row>
+    <row r="41" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A41" s="39">
+        <v>11.5</v>
+      </c>
+      <c r="B41" s="21" t="s">
+        <v>299</v>
+      </c>
+      <c r="C41" s="40" t="s">
+        <v>300</v>
+      </c>
+      <c r="D41" s="40" t="s">
+        <v>308</v>
+      </c>
+      <c r="E41" s="41"/>
+      <c r="F41" s="22"/>
+      <c r="G41" s="42"/>
+    </row>
+    <row r="42" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A42" s="39">
+        <v>11.51</v>
+      </c>
+      <c r="B42" s="21" t="s">
+        <v>240</v>
+      </c>
+      <c r="C42" s="40" t="s">
+        <v>301</v>
+      </c>
+      <c r="D42" s="40"/>
+      <c r="E42" s="41"/>
+      <c r="F42" s="22"/>
+      <c r="G42" s="42"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" s="7">
         <v>13</v>
       </c>
-      <c r="B41" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C41" s="8"/>
-      <c r="D41" s="7"/>
-      <c r="E41" s="9">
+      <c r="B43" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C43" s="8"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="9">
         <v>44045</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C42" s="4"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C43" s="4"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C44" s="4"/>
@@ -2624,6 +2697,12 @@
     </row>
     <row r="125" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C125" s="4"/>
+    </row>
+    <row r="126" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C126" s="4"/>
+    </row>
+    <row r="127" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C127" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2883,38 +2962,38 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
-        <v>141</v>
-      </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
+      <c r="A2" s="45" t="s">
+        <v>140</v>
+      </c>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
     </row>
     <row r="3" spans="1:8" s="11" customFormat="1" ht="38" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="C3" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="G3" s="15" t="s">
         <v>119</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>120</v>
       </c>
       <c r="H3" s="15" t="s">
         <v>25</v>
@@ -2922,210 +3001,210 @@
     </row>
     <row r="4" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>91</v>
-      </c>
       <c r="C4" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>91</v>
-      </c>
       <c r="C5" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="H5" s="10" t="s">
         <v>94</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="C6" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="G6" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="H6" s="10" t="s">
         <v>99</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>91</v>
-      </c>
       <c r="C7" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="H7" s="10" t="s">
         <v>101</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="61" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="B8" s="10" t="s">
-        <v>97</v>
-      </c>
       <c r="C8" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="57" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>91</v>
-      </c>
       <c r="C9" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="G9" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="H9" s="10" t="s">
         <v>106</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="G9" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="H9" s="10" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="C10" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="G10" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="H10" s="10" t="s">
         <v>111</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="G10" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="C11" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E11" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="E11" s="10" t="s">
+      <c r="F11" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="G11" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="F11" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="G11" s="18" t="s">
+      <c r="H11" s="10" t="s">
         <v>116</v>
-      </c>
-      <c r="H11" s="10" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="18" x14ac:dyDescent="0.2">
@@ -3149,38 +3228,38 @@
       <c r="H13" s="10"/>
     </row>
     <row r="14" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="24" t="s">
-        <v>149</v>
-      </c>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
+      <c r="A14" s="46" t="s">
+        <v>148</v>
+      </c>
+      <c r="B14" s="46"/>
+      <c r="C14" s="46"/>
+      <c r="D14" s="46"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="46"/>
+      <c r="H14" s="46"/>
     </row>
     <row r="15" spans="1:8" ht="38" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="B15" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="C15" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="G15" s="15" t="s">
         <v>119</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="F15" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="G15" s="15" t="s">
-        <v>120</v>
       </c>
       <c r="H15" s="15" t="s">
         <v>25</v>
@@ -3188,184 +3267,184 @@
     </row>
     <row r="16" spans="1:8" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="B16" s="17" t="s">
-        <v>91</v>
-      </c>
       <c r="C16" s="17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G16" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="H16" s="17" t="s">
         <v>150</v>
-      </c>
-      <c r="H16" s="17" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="B17" s="17" t="s">
-        <v>91</v>
-      </c>
       <c r="C17" s="17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D17" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="F17" s="20" t="s">
         <v>152</v>
       </c>
-      <c r="E17" s="17" t="s">
+      <c r="G17" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="F17" s="20" t="s">
-        <v>153</v>
-      </c>
-      <c r="G17" s="20" t="s">
+      <c r="H17" s="17" t="s">
         <v>156</v>
-      </c>
-      <c r="H17" s="17" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="18" spans="1:8" s="21" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="C18" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="G18" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="C18" s="17" t="s">
-        <v>147</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="E18" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="F18" s="20" t="s">
-        <v>146</v>
-      </c>
-      <c r="G18" s="20" t="s">
-        <v>92</v>
-      </c>
       <c r="H18" s="17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="B19" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="B19" s="17" t="s">
-        <v>97</v>
-      </c>
       <c r="C19" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F19" s="20" t="s">
+        <v>159</v>
+      </c>
+      <c r="G19" s="20" t="s">
         <v>160</v>
       </c>
-      <c r="G19" s="20" t="s">
+      <c r="H19" s="17" t="s">
         <v>161</v>
-      </c>
-      <c r="H19" s="17" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="60" x14ac:dyDescent="0.2">
       <c r="A20" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="B20" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="B20" s="17" t="s">
-        <v>91</v>
-      </c>
       <c r="C20" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F20" s="20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G20" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H20" s="17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A21" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="B21" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B21" s="17" t="s">
-        <v>109</v>
-      </c>
       <c r="C21" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F21" s="20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G21" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="H21" s="17" t="s">
         <v>166</v>
-      </c>
-      <c r="H21" s="17" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="B22" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="B22" s="17" t="s">
-        <v>114</v>
-      </c>
       <c r="C22" s="17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F22" s="20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G22" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="H22" s="17" t="s">
         <v>168</v>
-      </c>
-      <c r="H22" s="17" t="s">
-        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -3398,835 +3477,835 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="27" t="s">
+        <v>172</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>174</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>175</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>177</v>
+      </c>
+      <c r="H2" s="29" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="24" t="s">
+        <v>196</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="C3" s="23"/>
+      <c r="D3" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="E3" s="34" t="s">
+        <v>179</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="G3" s="34" t="s">
+        <v>179</v>
+      </c>
+      <c r="H3" s="25"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="24" t="s">
+        <v>232</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="23"/>
+      <c r="D4" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="G4" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="H4" s="25" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="24" t="s">
+        <v>197</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>181</v>
+      </c>
+      <c r="C5" s="23">
+        <v>255</v>
+      </c>
+      <c r="D5" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="G5" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="H5" s="25" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="24" t="s">
+        <v>233</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="C6" s="23"/>
+      <c r="D6" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="G6" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="H6" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="24" t="s">
+        <v>234</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>181</v>
+      </c>
+      <c r="C7" s="23">
+        <v>255</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="G7" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="H7" s="25"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="24" t="s">
+        <v>235</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="C8" s="23"/>
+      <c r="D8" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="F8" s="34" t="s">
+        <v>179</v>
+      </c>
+      <c r="G8" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="H8" s="25"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="24" t="s">
         <v>171</v>
       </c>
-      <c r="B1" s="28" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="29" t="s">
+      <c r="B9" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="C9" s="23"/>
+      <c r="D9" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="F9" s="34" t="s">
+        <v>179</v>
+      </c>
+      <c r="G9" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="H9" s="25"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="24" t="s">
+        <v>250</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="C10" s="23"/>
+      <c r="D10" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="F10" s="34" t="s">
+        <v>179</v>
+      </c>
+      <c r="G10" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="H10" s="25"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="C11" s="23"/>
+      <c r="D11" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="F11" s="34" t="s">
+        <v>179</v>
+      </c>
+      <c r="G11" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="H11" s="25"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="24" t="s">
+        <v>252</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="C12" s="23"/>
+      <c r="D12" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="F12" s="34" t="s">
+        <v>179</v>
+      </c>
+      <c r="G12" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="H12" s="25"/>
+    </row>
+    <row r="15" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="A15" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="27" t="s">
+        <v>172</v>
+      </c>
+      <c r="B16" s="28" t="s">
         <v>173</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="C16" s="28" t="s">
         <v>174</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="D16" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="E16" s="28" t="s">
         <v>175</v>
       </c>
-      <c r="D2" s="30" t="s">
-        <v>183</v>
-      </c>
-      <c r="E2" s="30" t="s">
+      <c r="F16" s="28" t="s">
         <v>176</v>
       </c>
-      <c r="F2" s="30" t="s">
+      <c r="G16" s="28" t="s">
         <v>177</v>
       </c>
-      <c r="G2" s="30" t="s">
+      <c r="H16" s="29" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="24" t="s">
+        <v>196</v>
+      </c>
+      <c r="B17" s="23" t="s">
         <v>178</v>
       </c>
-      <c r="H2" s="31" t="s">
+      <c r="C17" s="23"/>
+      <c r="D17" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="E17" s="34" t="s">
+        <v>179</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="G17" s="34" t="s">
+        <v>179</v>
+      </c>
+      <c r="H17" s="25"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="24" t="s">
+        <v>197</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>181</v>
+      </c>
+      <c r="C18" s="23">
+        <v>255</v>
+      </c>
+      <c r="D18" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="F18" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="G18" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="H18" s="25" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="24" t="s">
+        <v>218</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>220</v>
+      </c>
+      <c r="C19" s="23"/>
+      <c r="D19" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="G19" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="H19" s="25" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="26" t="s">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="24" t="s">
+        <v>219</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>220</v>
+      </c>
+      <c r="C20" s="23"/>
+      <c r="D20" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="G20" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="H20" s="25" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="A22" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="B22" s="26" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="27" t="s">
+        <v>172</v>
+      </c>
+      <c r="B23" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="C23" s="28" t="s">
+        <v>174</v>
+      </c>
+      <c r="D23" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="E23" s="28" t="s">
+        <v>175</v>
+      </c>
+      <c r="F23" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="G23" s="28" t="s">
+        <v>177</v>
+      </c>
+      <c r="H23" s="29" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="24" t="s">
+        <v>196</v>
+      </c>
+      <c r="B24" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="C24" s="23"/>
+      <c r="D24" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="E24" s="34" t="s">
+        <v>179</v>
+      </c>
+      <c r="F24" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="G24" s="34" t="s">
+        <v>179</v>
+      </c>
+      <c r="H24" s="25"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="24" t="s">
         <v>197</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B25" s="23" t="s">
+        <v>181</v>
+      </c>
+      <c r="C25" s="23">
+        <v>255</v>
+      </c>
+      <c r="D25" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="E25" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="F25" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="G25" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="H25" s="25" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="24" t="s">
+        <v>218</v>
+      </c>
+      <c r="B26" s="23" t="s">
+        <v>220</v>
+      </c>
+      <c r="C26" s="23"/>
+      <c r="D26" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="E26" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="F26" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="G26" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="H26" s="25" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="24" t="s">
+        <v>219</v>
+      </c>
+      <c r="B27" s="23" t="s">
+        <v>220</v>
+      </c>
+      <c r="C27" s="23"/>
+      <c r="D27" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="E27" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="F27" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="G27" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="H27" s="25" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="A29" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="B29" s="26" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="27" t="s">
+        <v>172</v>
+      </c>
+      <c r="B30" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="C30" s="28" t="s">
+        <v>174</v>
+      </c>
+      <c r="D30" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="E30" s="28" t="s">
+        <v>175</v>
+      </c>
+      <c r="F30" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="G30" s="28" t="s">
+        <v>177</v>
+      </c>
+      <c r="H30" s="29" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="24" t="s">
+        <v>196</v>
+      </c>
+      <c r="B31" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="C31" s="23"/>
+      <c r="D31" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="E31" s="34" t="s">
         <v>179</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="36" t="s">
+      <c r="F31" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="G31" s="34" t="s">
+        <v>179</v>
+      </c>
+      <c r="H31" s="25"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="24" t="s">
+        <v>197</v>
+      </c>
+      <c r="B32" s="23" t="s">
         <v>181</v>
       </c>
-      <c r="E3" s="36" t="s">
-        <v>180</v>
-      </c>
-      <c r="F3" s="25" t="s">
+      <c r="C32" s="23">
+        <v>255</v>
+      </c>
+      <c r="D32" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="E32" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="F32" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="G32" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="H32" s="25" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="24" t="s">
+        <v>218</v>
+      </c>
+      <c r="B33" s="23" t="s">
+        <v>220</v>
+      </c>
+      <c r="C33" s="23"/>
+      <c r="D33" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="E33" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="F33" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="G33" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="H33" s="25" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="24" t="s">
+        <v>219</v>
+      </c>
+      <c r="B34" s="23" t="s">
+        <v>220</v>
+      </c>
+      <c r="C34" s="23"/>
+      <c r="D34" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="E34" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="F34" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="G34" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="H34" s="25" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="A36" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="B36" s="26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="27" t="s">
+        <v>172</v>
+      </c>
+      <c r="B37" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="C37" s="28" t="s">
+        <v>174</v>
+      </c>
+      <c r="D37" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="E37" s="28" t="s">
+        <v>175</v>
+      </c>
+      <c r="F37" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="G37" s="28" t="s">
+        <v>177</v>
+      </c>
+      <c r="H37" s="29" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="24" t="s">
+        <v>196</v>
+      </c>
+      <c r="B38" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="C38" s="23"/>
+      <c r="D38" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="E38" s="34" t="s">
+        <v>179</v>
+      </c>
+      <c r="F38" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="G38" s="34" t="s">
+        <v>179</v>
+      </c>
+      <c r="H38" s="25"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="24" t="s">
+        <v>197</v>
+      </c>
+      <c r="B39" s="23" t="s">
         <v>181</v>
       </c>
-      <c r="G3" s="36" t="s">
-        <v>180</v>
-      </c>
-      <c r="H3" s="27"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="26" t="s">
-        <v>233</v>
-      </c>
-      <c r="B4" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="25"/>
-      <c r="D4" s="36" t="s">
+      <c r="C39" s="23">
+        <v>255</v>
+      </c>
+      <c r="D39" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="E39" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="F39" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="G39" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="H39" s="25" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="24" t="s">
+        <v>248</v>
+      </c>
+      <c r="B40" s="23" t="s">
         <v>181</v>
       </c>
-      <c r="E4" s="25" t="s">
+      <c r="C40" s="23">
+        <v>255</v>
+      </c>
+      <c r="D40" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="E40" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="F40" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="G40" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="H40" s="25"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="24" t="s">
+        <v>249</v>
+      </c>
+      <c r="B41" s="23" t="s">
         <v>181</v>
       </c>
-      <c r="F4" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="G4" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="H4" s="27" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="26" t="s">
-        <v>198</v>
-      </c>
-      <c r="B5" s="25" t="s">
-        <v>182</v>
-      </c>
-      <c r="C5" s="25">
+      <c r="C41" s="23">
         <v>255</v>
       </c>
-      <c r="D5" s="36" t="s">
-        <v>181</v>
-      </c>
-      <c r="E5" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="F5" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="G5" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="H5" s="27" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="26" t="s">
-        <v>234</v>
-      </c>
-      <c r="B6" s="25" t="s">
-        <v>188</v>
-      </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="36" t="s">
-        <v>181</v>
-      </c>
-      <c r="E6" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="F6" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="G6" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="H6" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="26" t="s">
-        <v>235</v>
-      </c>
-      <c r="B7" s="25" t="s">
-        <v>182</v>
-      </c>
-      <c r="C7" s="25">
-        <v>255</v>
-      </c>
-      <c r="D7" s="25" t="s">
-        <v>180</v>
-      </c>
-      <c r="E7" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="F7" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="G7" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="H7" s="27"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="B8" s="25" t="s">
+      <c r="D41" s="23" t="s">
         <v>179</v>
       </c>
-      <c r="C8" s="25"/>
-      <c r="D8" s="36" t="s">
-        <v>181</v>
-      </c>
-      <c r="E8" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="F8" s="36" t="s">
-        <v>180</v>
-      </c>
-      <c r="G8" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="H8" s="27"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="26" t="s">
-        <v>172</v>
-      </c>
-      <c r="B9" s="25" t="s">
-        <v>179</v>
-      </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="36" t="s">
-        <v>181</v>
-      </c>
-      <c r="E9" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="F9" s="36" t="s">
-        <v>180</v>
-      </c>
-      <c r="G9" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="H9" s="27"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="26" t="s">
-        <v>251</v>
-      </c>
-      <c r="B10" s="25" t="s">
-        <v>179</v>
-      </c>
-      <c r="C10" s="25"/>
-      <c r="D10" s="36" t="s">
-        <v>181</v>
-      </c>
-      <c r="E10" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="F10" s="36" t="s">
-        <v>180</v>
-      </c>
-      <c r="G10" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="H10" s="27"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="26" t="s">
-        <v>252</v>
-      </c>
-      <c r="B11" s="25" t="s">
-        <v>179</v>
-      </c>
-      <c r="C11" s="25"/>
-      <c r="D11" s="36" t="s">
-        <v>181</v>
-      </c>
-      <c r="E11" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="F11" s="36" t="s">
-        <v>180</v>
-      </c>
-      <c r="G11" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="H11" s="27"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="26" t="s">
-        <v>253</v>
-      </c>
-      <c r="B12" s="25" t="s">
-        <v>179</v>
-      </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="36" t="s">
-        <v>181</v>
-      </c>
-      <c r="E12" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="F12" s="36" t="s">
-        <v>180</v>
-      </c>
-      <c r="G12" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="H12" s="27"/>
-    </row>
-    <row r="15" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A15" s="28" t="s">
-        <v>171</v>
-      </c>
-      <c r="B15" s="28" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="29" t="s">
-        <v>173</v>
-      </c>
-      <c r="B16" s="30" t="s">
-        <v>174</v>
-      </c>
-      <c r="C16" s="30" t="s">
-        <v>175</v>
-      </c>
-      <c r="D16" s="30" t="s">
-        <v>183</v>
-      </c>
-      <c r="E16" s="30" t="s">
-        <v>176</v>
-      </c>
-      <c r="F16" s="30" t="s">
-        <v>177</v>
-      </c>
-      <c r="G16" s="30" t="s">
-        <v>178</v>
-      </c>
-      <c r="H16" s="31" t="s">
+      <c r="E41" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="F41" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="G41" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="H41" s="25"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" s="24" t="s">
+        <v>218</v>
+      </c>
+      <c r="B42" s="23" t="s">
+        <v>220</v>
+      </c>
+      <c r="C42" s="23"/>
+      <c r="D42" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="E42" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="F42" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="G42" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="H42" s="25" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="26" t="s">
-        <v>197</v>
-      </c>
-      <c r="B17" s="25" t="s">
-        <v>179</v>
-      </c>
-      <c r="C17" s="25"/>
-      <c r="D17" s="36" t="s">
-        <v>181</v>
-      </c>
-      <c r="E17" s="36" t="s">
-        <v>180</v>
-      </c>
-      <c r="F17" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="G17" s="36" t="s">
-        <v>180</v>
-      </c>
-      <c r="H17" s="27"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="26" t="s">
-        <v>198</v>
-      </c>
-      <c r="B18" s="25" t="s">
-        <v>182</v>
-      </c>
-      <c r="C18" s="25">
-        <v>255</v>
-      </c>
-      <c r="D18" s="36" t="s">
-        <v>181</v>
-      </c>
-      <c r="E18" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="F18" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="G18" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="H18" s="27" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="26" t="s">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" s="24" t="s">
         <v>219</v>
       </c>
-      <c r="B19" s="25" t="s">
-        <v>221</v>
-      </c>
-      <c r="C19" s="25"/>
-      <c r="D19" s="36" t="s">
-        <v>181</v>
-      </c>
-      <c r="E19" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="F19" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="G19" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="H19" s="27" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="26" t="s">
+      <c r="B43" s="23" t="s">
         <v>220</v>
       </c>
-      <c r="B20" s="25" t="s">
-        <v>221</v>
-      </c>
-      <c r="C20" s="25"/>
-      <c r="D20" s="36" t="s">
-        <v>181</v>
-      </c>
-      <c r="E20" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="F20" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="G20" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="H20" s="27" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A22" s="28" t="s">
-        <v>171</v>
-      </c>
-      <c r="B22" s="28" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="29" t="s">
-        <v>173</v>
-      </c>
-      <c r="B23" s="30" t="s">
-        <v>174</v>
-      </c>
-      <c r="C23" s="30" t="s">
-        <v>175</v>
-      </c>
-      <c r="D23" s="30" t="s">
-        <v>183</v>
-      </c>
-      <c r="E23" s="30" t="s">
-        <v>176</v>
-      </c>
-      <c r="F23" s="30" t="s">
-        <v>177</v>
-      </c>
-      <c r="G23" s="30" t="s">
-        <v>178</v>
-      </c>
-      <c r="H23" s="31" t="s">
+      <c r="C43" s="23"/>
+      <c r="D43" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="E43" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="F43" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="G43" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="H43" s="25" t="s">
         <v>189</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="26" t="s">
-        <v>197</v>
-      </c>
-      <c r="B24" s="25" t="s">
-        <v>179</v>
-      </c>
-      <c r="C24" s="25"/>
-      <c r="D24" s="36" t="s">
-        <v>181</v>
-      </c>
-      <c r="E24" s="36" t="s">
-        <v>180</v>
-      </c>
-      <c r="F24" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="G24" s="36" t="s">
-        <v>180</v>
-      </c>
-      <c r="H24" s="27"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="26" t="s">
-        <v>198</v>
-      </c>
-      <c r="B25" s="25" t="s">
-        <v>182</v>
-      </c>
-      <c r="C25" s="25">
-        <v>255</v>
-      </c>
-      <c r="D25" s="36" t="s">
-        <v>181</v>
-      </c>
-      <c r="E25" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="F25" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="G25" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="H25" s="27" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="26" t="s">
-        <v>219</v>
-      </c>
-      <c r="B26" s="25" t="s">
-        <v>221</v>
-      </c>
-      <c r="C26" s="25"/>
-      <c r="D26" s="36" t="s">
-        <v>181</v>
-      </c>
-      <c r="E26" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="F26" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="G26" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="H26" s="27" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="26" t="s">
-        <v>220</v>
-      </c>
-      <c r="B27" s="25" t="s">
-        <v>221</v>
-      </c>
-      <c r="C27" s="25"/>
-      <c r="D27" s="36" t="s">
-        <v>181</v>
-      </c>
-      <c r="E27" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="F27" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="G27" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="H27" s="27" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A29" s="28" t="s">
-        <v>171</v>
-      </c>
-      <c r="B29" s="28" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="29" t="s">
-        <v>173</v>
-      </c>
-      <c r="B30" s="30" t="s">
-        <v>174</v>
-      </c>
-      <c r="C30" s="30" t="s">
-        <v>175</v>
-      </c>
-      <c r="D30" s="30" t="s">
-        <v>183</v>
-      </c>
-      <c r="E30" s="30" t="s">
-        <v>176</v>
-      </c>
-      <c r="F30" s="30" t="s">
-        <v>177</v>
-      </c>
-      <c r="G30" s="30" t="s">
-        <v>178</v>
-      </c>
-      <c r="H30" s="31" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="26" t="s">
-        <v>197</v>
-      </c>
-      <c r="B31" s="25" t="s">
-        <v>179</v>
-      </c>
-      <c r="C31" s="25"/>
-      <c r="D31" s="36" t="s">
-        <v>181</v>
-      </c>
-      <c r="E31" s="36" t="s">
-        <v>180</v>
-      </c>
-      <c r="F31" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="G31" s="36" t="s">
-        <v>180</v>
-      </c>
-      <c r="H31" s="27"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="26" t="s">
-        <v>198</v>
-      </c>
-      <c r="B32" s="25" t="s">
-        <v>182</v>
-      </c>
-      <c r="C32" s="25">
-        <v>255</v>
-      </c>
-      <c r="D32" s="36" t="s">
-        <v>181</v>
-      </c>
-      <c r="E32" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="F32" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="G32" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="H32" s="27" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="26" t="s">
-        <v>219</v>
-      </c>
-      <c r="B33" s="25" t="s">
-        <v>221</v>
-      </c>
-      <c r="C33" s="25"/>
-      <c r="D33" s="36" t="s">
-        <v>181</v>
-      </c>
-      <c r="E33" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="F33" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="G33" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="H33" s="27" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="26" t="s">
-        <v>220</v>
-      </c>
-      <c r="B34" s="25" t="s">
-        <v>221</v>
-      </c>
-      <c r="C34" s="25"/>
-      <c r="D34" s="36" t="s">
-        <v>181</v>
-      </c>
-      <c r="E34" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="F34" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="G34" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="H34" s="27" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A36" s="28" t="s">
-        <v>171</v>
-      </c>
-      <c r="B36" s="28" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="29" t="s">
-        <v>173</v>
-      </c>
-      <c r="B37" s="30" t="s">
-        <v>174</v>
-      </c>
-      <c r="C37" s="30" t="s">
-        <v>175</v>
-      </c>
-      <c r="D37" s="30" t="s">
-        <v>183</v>
-      </c>
-      <c r="E37" s="30" t="s">
-        <v>176</v>
-      </c>
-      <c r="F37" s="30" t="s">
-        <v>177</v>
-      </c>
-      <c r="G37" s="30" t="s">
-        <v>178</v>
-      </c>
-      <c r="H37" s="31" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="26" t="s">
-        <v>197</v>
-      </c>
-      <c r="B38" s="25" t="s">
-        <v>179</v>
-      </c>
-      <c r="C38" s="25"/>
-      <c r="D38" s="36" t="s">
-        <v>181</v>
-      </c>
-      <c r="E38" s="36" t="s">
-        <v>180</v>
-      </c>
-      <c r="F38" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="G38" s="36" t="s">
-        <v>180</v>
-      </c>
-      <c r="H38" s="27"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="26" t="s">
-        <v>198</v>
-      </c>
-      <c r="B39" s="25" t="s">
-        <v>182</v>
-      </c>
-      <c r="C39" s="25">
-        <v>255</v>
-      </c>
-      <c r="D39" s="36" t="s">
-        <v>181</v>
-      </c>
-      <c r="E39" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="F39" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="G39" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="H39" s="27" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="26" t="s">
-        <v>249</v>
-      </c>
-      <c r="B40" s="25" t="s">
-        <v>182</v>
-      </c>
-      <c r="C40" s="25">
-        <v>255</v>
-      </c>
-      <c r="D40" s="25" t="s">
-        <v>180</v>
-      </c>
-      <c r="E40" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="F40" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="G40" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="H40" s="27"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="26" t="s">
-        <v>250</v>
-      </c>
-      <c r="B41" s="25" t="s">
-        <v>182</v>
-      </c>
-      <c r="C41" s="25">
-        <v>255</v>
-      </c>
-      <c r="D41" s="25" t="s">
-        <v>180</v>
-      </c>
-      <c r="E41" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="F41" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="G41" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="H41" s="27"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A42" s="26" t="s">
-        <v>219</v>
-      </c>
-      <c r="B42" s="25" t="s">
-        <v>221</v>
-      </c>
-      <c r="C42" s="25"/>
-      <c r="D42" s="36" t="s">
-        <v>181</v>
-      </c>
-      <c r="E42" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="F42" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="G42" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="H42" s="27" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A43" s="26" t="s">
-        <v>220</v>
-      </c>
-      <c r="B43" s="25" t="s">
-        <v>221</v>
-      </c>
-      <c r="C43" s="25"/>
-      <c r="D43" s="36" t="s">
-        <v>181</v>
-      </c>
-      <c r="E43" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="F43" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="G43" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="H43" s="27" t="s">
-        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -4238,8 +4317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{548A6984-5372-3942-B42C-A3C7DE1E5AD2}">
   <dimension ref="A2:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4258,310 +4337,310 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:2" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="27" t="s">
+        <v>196</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="24">
+        <v>1</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="24">
+        <v>2</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="24">
+        <v>3</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="24">
+        <v>4</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="24">
+        <v>5</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="A10" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="27" t="s">
+        <v>196</v>
+      </c>
+      <c r="B11" s="28" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="24">
+        <v>1</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="24">
+        <v>2</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="24">
+        <v>3</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="24">
+        <v>4</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="24">
+        <v>5</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="24">
+        <v>6</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="24">
+        <v>7</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="24">
+        <v>8</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="35"/>
+      <c r="B20" s="35"/>
+    </row>
+    <row r="21" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A21" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="27" t="s">
+        <v>196</v>
+      </c>
+      <c r="B22" s="28" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="24">
+        <v>1</v>
+      </c>
+      <c r="B23" s="23" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="24">
+        <v>2</v>
+      </c>
+      <c r="B24" s="23" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="24">
+        <v>3</v>
+      </c>
+      <c r="B25" s="23" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="24">
+        <v>4</v>
+      </c>
+      <c r="B26" s="23" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="24">
+        <v>5</v>
+      </c>
+      <c r="B27" s="23" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="35"/>
+      <c r="B28" s="35"/>
+    </row>
+    <row r="29" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A29" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="B29" s="26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="27" t="s">
+        <v>196</v>
+      </c>
+      <c r="B30" s="28" t="s">
+        <v>197</v>
+      </c>
+      <c r="C30" s="28" t="s">
+        <v>248</v>
+      </c>
+      <c r="D30" s="28" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="24">
+        <v>1</v>
+      </c>
+      <c r="B31" s="23" t="s">
+        <v>278</v>
+      </c>
+      <c r="C31" s="23" t="s">
+        <v>276</v>
+      </c>
+      <c r="D31" s="23" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="24">
+        <v>2</v>
+      </c>
+      <c r="B32" s="23" t="s">
+        <v>272</v>
+      </c>
+      <c r="C32" s="23" t="s">
+        <v>273</v>
+      </c>
+      <c r="D32" s="23" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+      <c r="A34" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="B34" s="26" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" s="27" t="s">
+        <v>196</v>
+      </c>
+      <c r="B35" s="28" t="s">
+        <v>232</v>
+      </c>
+      <c r="C35" s="28" t="s">
+        <v>197</v>
+      </c>
+      <c r="D35" s="28" t="s">
+        <v>233</v>
+      </c>
+      <c r="E35" s="28" t="s">
+        <v>234</v>
+      </c>
+      <c r="F35" s="28" t="s">
+        <v>235</v>
+      </c>
+      <c r="G35" s="28" t="s">
         <v>171</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="29" t="s">
-        <v>197</v>
-      </c>
-      <c r="B3" s="30" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="26">
-        <v>1</v>
-      </c>
-      <c r="B4" s="25" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="26">
-        <v>2</v>
-      </c>
-      <c r="B5" s="25" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="26">
-        <v>3</v>
-      </c>
-      <c r="B6" s="25" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="26">
-        <v>4</v>
-      </c>
-      <c r="B7" s="25" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="26">
-        <v>5</v>
-      </c>
-      <c r="B8" s="25" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="21" x14ac:dyDescent="0.25">
-      <c r="A10" s="28" t="s">
-        <v>171</v>
-      </c>
-      <c r="B10" s="28" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="29" t="s">
-        <v>197</v>
-      </c>
-      <c r="B11" s="30" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="26">
-        <v>1</v>
-      </c>
-      <c r="B12" s="25" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="26">
-        <v>2</v>
-      </c>
-      <c r="B13" s="25" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="26">
-        <v>3</v>
-      </c>
-      <c r="B14" s="25" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="26">
-        <v>4</v>
-      </c>
-      <c r="B15" s="25" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="26">
-        <v>5</v>
-      </c>
-      <c r="B16" s="25" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="26">
-        <v>6</v>
-      </c>
-      <c r="B17" s="25" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="26">
-        <v>7</v>
-      </c>
-      <c r="B18" s="25" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="26">
-        <v>8</v>
-      </c>
-      <c r="B19" s="25" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="37"/>
-      <c r="B20" s="37"/>
-    </row>
-    <row r="21" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A21" s="28" t="s">
-        <v>171</v>
-      </c>
-      <c r="B21" s="28" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="29" t="s">
-        <v>197</v>
-      </c>
-      <c r="B22" s="30" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="26">
-        <v>1</v>
-      </c>
-      <c r="B23" s="25" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="26">
-        <v>2</v>
-      </c>
-      <c r="B24" s="25" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="26">
-        <v>3</v>
-      </c>
-      <c r="B25" s="25" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="26">
-        <v>4</v>
-      </c>
-      <c r="B26" s="25" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="26">
-        <v>5</v>
-      </c>
-      <c r="B27" s="25" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="37"/>
-      <c r="B28" s="37"/>
-    </row>
-    <row r="29" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A29" s="28" t="s">
-        <v>171</v>
-      </c>
-      <c r="B29" s="28" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="29" t="s">
-        <v>197</v>
-      </c>
-      <c r="B30" s="30" t="s">
-        <v>198</v>
-      </c>
-      <c r="C30" s="30" t="s">
-        <v>249</v>
-      </c>
-      <c r="D30" s="30" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="26">
-        <v>1</v>
-      </c>
-      <c r="B31" s="25" t="s">
-        <v>279</v>
-      </c>
-      <c r="C31" s="25" t="s">
-        <v>277</v>
-      </c>
-      <c r="D31" s="25" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="26">
-        <v>2</v>
-      </c>
-      <c r="B32" s="25" t="s">
-        <v>273</v>
-      </c>
-      <c r="C32" s="25" t="s">
-        <v>274</v>
-      </c>
-      <c r="D32" s="25" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="A34" s="28" t="s">
-        <v>171</v>
-      </c>
-      <c r="B34" s="28" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A35" s="29" t="s">
-        <v>197</v>
-      </c>
-      <c r="B35" s="30" t="s">
-        <v>233</v>
-      </c>
-      <c r="C35" s="30" t="s">
-        <v>198</v>
-      </c>
-      <c r="D35" s="30" t="s">
-        <v>234</v>
-      </c>
-      <c r="E35" s="30" t="s">
-        <v>235</v>
-      </c>
-      <c r="F35" s="30" t="s">
-        <v>236</v>
-      </c>
-      <c r="G35" s="30" t="s">
-        <v>172</v>
-      </c>
-      <c r="H35" s="30" t="s">
+      <c r="H35" s="28" t="s">
+        <v>250</v>
+      </c>
+      <c r="I35" s="28" t="s">
         <v>251</v>
       </c>
-      <c r="I35" s="30" t="s">
+      <c r="J35" s="28" t="s">
         <v>252</v>
-      </c>
-      <c r="J35" s="30" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>1</v>
       </c>
-      <c r="B36" s="47" t="s">
-        <v>291</v>
+      <c r="B36" s="44" t="s">
+        <v>290</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="D36" s="38">
+        <v>280</v>
+      </c>
+      <c r="D36" s="36">
         <v>120</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F36" s="1">
         <v>1</v>
@@ -4583,13 +4662,13 @@
       <c r="A37" s="1">
         <v>2</v>
       </c>
-      <c r="B37" s="47" t="s">
-        <v>292</v>
+      <c r="B37" s="44" t="s">
+        <v>291</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D37" s="38">
+        <v>281</v>
+      </c>
+      <c r="D37" s="36">
         <v>20</v>
       </c>
       <c r="F37" s="1">
@@ -4612,13 +4691,13 @@
       <c r="A38" s="1">
         <v>3</v>
       </c>
-      <c r="B38" s="47" t="s">
-        <v>292</v>
+      <c r="B38" s="44" t="s">
+        <v>291</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="D38" s="38">
+        <v>282</v>
+      </c>
+      <c r="D38" s="36">
         <v>40</v>
       </c>
       <c r="F38" s="1">
@@ -4641,13 +4720,13 @@
       <c r="A39" s="1">
         <v>4</v>
       </c>
-      <c r="B39" s="47" t="s">
-        <v>293</v>
+      <c r="B39" s="44" t="s">
+        <v>292</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="D39" s="38">
+        <v>283</v>
+      </c>
+      <c r="D39" s="36">
         <v>150</v>
       </c>
       <c r="F39" s="1">
@@ -4670,13 +4749,13 @@
       <c r="A40" s="1">
         <v>5</v>
       </c>
-      <c r="B40" s="47" t="s">
-        <v>293</v>
+      <c r="B40" s="44" t="s">
+        <v>292</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D40" s="38">
+        <v>284</v>
+      </c>
+      <c r="D40" s="36">
         <v>20</v>
       </c>
       <c r="F40" s="1">
@@ -4699,17 +4778,17 @@
       <c r="A41" s="1">
         <v>6</v>
       </c>
-      <c r="B41" s="47" t="s">
-        <v>293</v>
+      <c r="B41" s="44" t="s">
+        <v>292</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D41" s="38">
-        <v>80</v>
+        <v>285</v>
+      </c>
+      <c r="D41" s="36">
+        <v>80.5</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F41" s="1">
         <v>1</v>
@@ -4731,14 +4810,17 @@
       <c r="A42" s="1">
         <v>7</v>
       </c>
-      <c r="B42" s="47" t="s">
-        <v>280</v>
+      <c r="B42" s="44" t="s">
+        <v>279</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="D42" s="38">
+        <v>286</v>
+      </c>
+      <c r="D42" s="36">
         <v>500</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>298</v>
       </c>
       <c r="F42" s="1">
         <v>1</v>
@@ -4760,14 +4842,17 @@
       <c r="A43" s="1">
         <v>8</v>
       </c>
-      <c r="B43" s="47" t="s">
-        <v>294</v>
+      <c r="B43" s="44" t="s">
+        <v>293</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="D43" s="38">
+        <v>287</v>
+      </c>
+      <c r="D43" s="36">
         <v>300</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>298</v>
       </c>
       <c r="F43" s="1">
         <v>1</v>
@@ -4789,17 +4874,17 @@
       <c r="A44" s="1">
         <v>9</v>
       </c>
-      <c r="B44" s="47" t="s">
-        <v>294</v>
+      <c r="B44" s="44" t="s">
+        <v>293</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="D44" s="38">
+        <v>288</v>
+      </c>
+      <c r="D44" s="36">
         <v>800</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F44" s="1">
         <v>1</v>
@@ -4821,13 +4906,13 @@
       <c r="A45" s="1">
         <v>10</v>
       </c>
-      <c r="B45" s="47" t="s">
-        <v>295</v>
+      <c r="B45" s="44" t="s">
+        <v>294</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="D45" s="38">
+        <v>289</v>
+      </c>
+      <c r="D45" s="36">
         <v>120</v>
       </c>
       <c r="F45" s="1">

</xml_diff>

<commit_message>
Commit: MVP ready Styling not complete
</commit_message>
<xml_diff>
--- a/documentation/Expense_Tracker_App_plan.xlsx
+++ b/documentation/Expense_Tracker_App_plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ct08284/sei/projects/deere-project2-starter/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA0332CE-FD68-2B4B-9E38-3BAE4A629BD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF7DBFA6-BA66-764C-BCD7-83C78B2B9956}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" xr2:uid="{05595CE3-5133-A840-8AB2-952878BB912B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" activeTab="5" xr2:uid="{05595CE3-5133-A840-8AB2-952878BB912B}"/>
   </bookViews>
   <sheets>
     <sheet name="Development_plan" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="318">
   <si>
     <t>Feature #</t>
   </si>
@@ -281,9 +281,6 @@
   </si>
   <si>
     <t>Excel</t>
-  </si>
-  <si>
-    <t>DEFINE REST OF THE PLAN</t>
   </si>
   <si>
     <t>Wireframing</t>
@@ -994,6 +991,38 @@
   </si>
   <si>
     <t>seeders/timestamp-demo-expenses.js</t>
+  </si>
+  <si>
+    <t>Work on Expenses controller</t>
+  </si>
+  <si>
+    <t>Create expensesController.js</t>
+  </si>
+  <si>
+    <t>Create file in controllers/expensesController.js</t>
+  </si>
+  <si>
+    <t>- Ini the file comparing with fruitsController.js
+- No routes still</t>
+  </si>
+  <si>
+    <t>Update server.js</t>
+  </si>
+  <si>
+    <t>Update file /server.js</t>
+  </si>
+  <si>
+    <t>- Include app.use for cookieParser
+- Include app.use for expenses</t>
+  </si>
+  <si>
+    <t>Create index.js for expenses</t>
+  </si>
+  <si>
+    <t>Create file /views/expenses/index.js</t>
+  </si>
+  <si>
+    <t>- Start with fruits.js code</t>
   </si>
 </sst>
 </file>
@@ -1066,7 +1095,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1076,12 +1105,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1191,7 +1214,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1203,11 +1226,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="15" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
@@ -1236,37 +1254,37 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="1" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1279,15 +1297,18 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1604,10 +1625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FFC9C39-9695-8A40-8D81-C0586B568F96}">
-  <dimension ref="A1:G127"/>
+  <dimension ref="A1:G121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1656,8 +1677,8 @@
       <c r="E2" s="6">
         <v>44043</v>
       </c>
-      <c r="F2" s="22" t="s">
-        <v>85</v>
+      <c r="F2" s="19" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -1671,8 +1692,8 @@
       <c r="E3" s="6">
         <v>44043</v>
       </c>
-      <c r="F3" s="22" t="s">
-        <v>85</v>
+      <c r="F3" s="19" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -1686,11 +1707,11 @@
       <c r="E4" s="6">
         <v>44044</v>
       </c>
-      <c r="F4" s="22" t="s">
-        <v>85</v>
+      <c r="F4" s="19" t="s">
+        <v>84</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -1704,11 +1725,11 @@
       <c r="E5" s="6">
         <v>44044</v>
       </c>
-      <c r="F5" s="22" t="s">
-        <v>85</v>
+      <c r="F5" s="19" t="s">
+        <v>84</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1724,8 +1745,8 @@
       <c r="E6" s="6">
         <v>44044</v>
       </c>
-      <c r="F6" s="30" t="s">
-        <v>86</v>
+      <c r="F6" s="27" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -1733,22 +1754,22 @@
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="D7" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="E7" s="6">
         <v>44045</v>
       </c>
-      <c r="F7" s="22" t="s">
-        <v>85</v>
+      <c r="F7" s="19" t="s">
+        <v>84</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1767,8 +1788,8 @@
       <c r="E8" s="6">
         <v>44045</v>
       </c>
-      <c r="F8" s="22" t="s">
-        <v>85</v>
+      <c r="F8" s="19" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1787,27 +1808,27 @@
       <c r="E9" s="6">
         <v>44045</v>
       </c>
-      <c r="F9" s="22" t="s">
-        <v>85</v>
+      <c r="F9" s="19" t="s">
+        <v>84</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="31">
+      <c r="A10" s="28">
         <v>9</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="33">
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="30">
         <v>44045</v>
       </c>
-      <c r="F10" s="22" t="s">
-        <v>85</v>
+      <c r="F10" s="19" t="s">
+        <v>84</v>
       </c>
       <c r="G10" s="5"/>
     </row>
@@ -1816,17 +1837,17 @@
         <v>9.1</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>192</v>
-      </c>
       <c r="E11" s="6"/>
-      <c r="F11" s="22" t="s">
-        <v>85</v>
+      <c r="F11" s="19" t="s">
+        <v>84</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>31</v>
@@ -1837,15 +1858,15 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E12" s="6"/>
-      <c r="F12" s="22" t="s">
-        <v>85</v>
+      <c r="F12" s="19" t="s">
+        <v>84</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>31</v>
@@ -1856,15 +1877,15 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E13" s="6"/>
-      <c r="F13" s="22" t="s">
-        <v>85</v>
+      <c r="F13" s="19" t="s">
+        <v>84</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>31</v>
@@ -1875,15 +1896,15 @@
         <v>9.4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E14" s="6"/>
-      <c r="F14" s="22" t="s">
-        <v>85</v>
+      <c r="F14" s="19" t="s">
+        <v>84</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>31</v>
@@ -1894,53 +1915,53 @@
         <v>9.5</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E15" s="6"/>
-      <c r="F15" s="22" t="s">
-        <v>85</v>
+      <c r="F15" s="19" t="s">
+        <v>84</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="38">
+      <c r="A16" s="35">
         <v>10</v>
       </c>
-      <c r="B16" s="31" t="s">
-        <v>214</v>
-      </c>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="33">
+      <c r="B16" s="28" t="s">
+        <v>213</v>
+      </c>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="30">
         <v>44045</v>
       </c>
-      <c r="F16" s="37" t="s">
-        <v>87</v>
+      <c r="F16" s="34" t="s">
+        <v>86</v>
       </c>
       <c r="G16" s="5"/>
     </row>
     <row r="17" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="36">
+      <c r="A17" s="33">
         <v>10.1</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>75</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E17" s="6"/>
-      <c r="F17" s="22" t="s">
-        <v>85</v>
+      <c r="F17" s="19" t="s">
+        <v>84</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>31</v>
@@ -1951,17 +1972,17 @@
         <v>10.11</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>75</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E18" s="6"/>
-      <c r="F18" s="22" t="s">
-        <v>85</v>
+      <c r="F18" s="19" t="s">
+        <v>84</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>31</v>
@@ -1972,38 +1993,38 @@
         <v>10.119999999999999</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>78</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E19" s="6"/>
-      <c r="F19" s="22" t="s">
-        <v>85</v>
+      <c r="F19" s="19" t="s">
+        <v>84</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="36">
+      <c r="A20" s="33">
         <v>10.199999999999999</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>75</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E20" s="6"/>
-      <c r="F20" s="22" t="s">
-        <v>85</v>
+      <c r="F20" s="19" t="s">
+        <v>84</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>31</v>
@@ -2014,17 +2035,17 @@
         <v>10.210000000000001</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>75</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E21" s="6"/>
-      <c r="F21" s="22" t="s">
-        <v>85</v>
+      <c r="F21" s="19" t="s">
+        <v>84</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>31</v>
@@ -2035,38 +2056,38 @@
         <v>10.220000000000001</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>78</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E22" s="6"/>
-      <c r="F22" s="22" t="s">
-        <v>85</v>
+      <c r="F22" s="19" t="s">
+        <v>84</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="36">
+      <c r="A23" s="33">
         <v>10.3</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>75</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E23" s="6"/>
-      <c r="F23" s="22" t="s">
-        <v>85</v>
+      <c r="F23" s="19" t="s">
+        <v>84</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>31</v>
@@ -2077,17 +2098,17 @@
         <v>10.31</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>75</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E24" s="6"/>
-      <c r="F24" s="22" t="s">
-        <v>85</v>
+      <c r="F24" s="19" t="s">
+        <v>84</v>
       </c>
       <c r="G24" s="5" t="s">
         <v>31</v>
@@ -2098,38 +2119,38 @@
         <v>10.32</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>78</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E25" s="6"/>
-      <c r="F25" s="22" t="s">
-        <v>85</v>
+      <c r="F25" s="19" t="s">
+        <v>84</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="36">
+      <c r="A26" s="33">
         <v>10.4</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>75</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E26" s="6"/>
-      <c r="F26" s="22" t="s">
-        <v>85</v>
+      <c r="F26" s="19" t="s">
+        <v>84</v>
       </c>
       <c r="G26" s="5" t="s">
         <v>31</v>
@@ -2140,17 +2161,17 @@
         <v>10.41</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>75</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E27" s="6"/>
-      <c r="F27" s="22" t="s">
-        <v>85</v>
+      <c r="F27" s="19" t="s">
+        <v>84</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>31</v>
@@ -2161,41 +2182,41 @@
         <v>10.42</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>78</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E28" s="6"/>
-      <c r="F28" s="22" t="s">
-        <v>85</v>
+      <c r="F28" s="19" t="s">
+        <v>84</v>
       </c>
       <c r="G28" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="36">
+      <c r="A29" s="33">
         <v>10.5</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>75</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E29" s="6"/>
-      <c r="F29" s="22" t="s">
-        <v>85</v>
+      <c r="F29" s="19" t="s">
+        <v>84</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -2203,17 +2224,17 @@
         <v>10.51</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>75</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E30" s="6"/>
-      <c r="F30" s="22" t="s">
-        <v>85</v>
+      <c r="F30" s="19" t="s">
+        <v>84</v>
       </c>
       <c r="G30" s="5" t="s">
         <v>31</v>
@@ -2224,242 +2245,285 @@
         <v>10.52</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>78</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E31" s="6"/>
-      <c r="F31" s="22" t="s">
-        <v>85</v>
+      <c r="F31" s="19" t="s">
+        <v>84</v>
       </c>
       <c r="G31" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="38">
+      <c r="A32" s="35">
         <v>11</v>
       </c>
-      <c r="B32" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="C32" s="32"/>
-      <c r="D32" s="32"/>
-      <c r="E32" s="33">
+      <c r="B32" s="28" t="s">
+        <v>236</v>
+      </c>
+      <c r="C32" s="29"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="30">
         <v>44045</v>
       </c>
-      <c r="F32" s="43" t="s">
-        <v>86</v>
+      <c r="F32" s="19" t="s">
+        <v>84</v>
       </c>
       <c r="G32" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A33" s="39">
+      <c r="A33" s="36">
         <v>11.1</v>
       </c>
-      <c r="B33" s="21" t="s">
-        <v>238</v>
-      </c>
-      <c r="C33" s="40" t="s">
-        <v>243</v>
-      </c>
-      <c r="D33" s="40" t="s">
-        <v>247</v>
-      </c>
-      <c r="E33" s="41"/>
-      <c r="F33" s="22" t="s">
-        <v>85</v>
+      <c r="B33" s="18" t="s">
+        <v>237</v>
+      </c>
+      <c r="C33" s="37" t="s">
+        <v>242</v>
+      </c>
+      <c r="D33" s="37" t="s">
+        <v>246</v>
+      </c>
+      <c r="E33" s="38"/>
+      <c r="F33" s="19" t="s">
+        <v>84</v>
       </c>
       <c r="G33" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="68" x14ac:dyDescent="0.2">
-      <c r="A34" s="39">
+      <c r="A34" s="36">
         <v>11.11</v>
       </c>
-      <c r="B34" s="21" t="s">
-        <v>240</v>
-      </c>
-      <c r="C34" s="40" t="s">
-        <v>305</v>
-      </c>
-      <c r="D34" s="40"/>
-      <c r="E34" s="41"/>
-      <c r="F34" s="22" t="s">
-        <v>85</v>
+      <c r="B34" s="18" t="s">
+        <v>239</v>
+      </c>
+      <c r="C34" s="37" t="s">
+        <v>304</v>
+      </c>
+      <c r="D34" s="37"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="19" t="s">
+        <v>84</v>
       </c>
       <c r="G34" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A35" s="39">
+      <c r="A35" s="36">
         <v>11.2</v>
       </c>
-      <c r="B35" s="21" t="s">
+      <c r="B35" s="18" t="s">
+        <v>238</v>
+      </c>
+      <c r="C35" s="37" t="s">
+        <v>243</v>
+      </c>
+      <c r="D35" s="37" t="s">
+        <v>252</v>
+      </c>
+      <c r="E35" s="38"/>
+      <c r="F35" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="G35" s="39"/>
+    </row>
+    <row r="36" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A36" s="36">
+        <v>11.21</v>
+      </c>
+      <c r="B36" s="18" t="s">
         <v>239</v>
       </c>
-      <c r="C35" s="40" t="s">
+      <c r="C36" s="37" t="s">
+        <v>303</v>
+      </c>
+      <c r="D36" s="37"/>
+      <c r="E36" s="38"/>
+      <c r="F36" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="G36" s="39"/>
+    </row>
+    <row r="37" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" s="36">
+        <v>11.3</v>
+      </c>
+      <c r="B37" s="18" t="s">
+        <v>240</v>
+      </c>
+      <c r="C37" s="37" t="s">
         <v>244</v>
       </c>
-      <c r="D35" s="40" t="s">
-        <v>253</v>
-      </c>
-      <c r="E35" s="41"/>
-      <c r="F35" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="G35" s="42"/>
-    </row>
-    <row r="36" spans="1:7" ht="68" x14ac:dyDescent="0.2">
-      <c r="A36" s="39">
-        <v>11.21</v>
-      </c>
-      <c r="B36" s="21" t="s">
-        <v>240</v>
-      </c>
-      <c r="C36" s="40" t="s">
-        <v>304</v>
-      </c>
-      <c r="D36" s="40"/>
-      <c r="E36" s="41"/>
-      <c r="F36" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="G36" s="42"/>
-    </row>
-    <row r="37" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" s="39">
-        <v>11.3</v>
-      </c>
-      <c r="B37" s="21" t="s">
+      <c r="D37" s="37" t="s">
+        <v>305</v>
+      </c>
+      <c r="E37" s="38"/>
+      <c r="F37" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="G37" s="39"/>
+    </row>
+    <row r="38" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A38" s="36">
+        <v>11.31</v>
+      </c>
+      <c r="B38" s="18" t="s">
+        <v>239</v>
+      </c>
+      <c r="C38" s="37" t="s">
+        <v>302</v>
+      </c>
+      <c r="D38" s="37"/>
+      <c r="E38" s="38"/>
+      <c r="F38" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="G38" s="39"/>
+    </row>
+    <row r="39" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A39" s="36">
+        <v>11.4</v>
+      </c>
+      <c r="B39" s="18" t="s">
         <v>241</v>
       </c>
-      <c r="C37" s="40" t="s">
+      <c r="C39" s="37" t="s">
         <v>245</v>
       </c>
-      <c r="D37" s="40" t="s">
+      <c r="D39" s="37" t="s">
         <v>306</v>
       </c>
-      <c r="E37" s="41"/>
-      <c r="F37" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="G37" s="42"/>
-    </row>
-    <row r="38" spans="1:7" ht="68" x14ac:dyDescent="0.2">
-      <c r="A38" s="39">
-        <v>11.31</v>
-      </c>
-      <c r="B38" s="21" t="s">
-        <v>240</v>
-      </c>
-      <c r="C38" s="40" t="s">
-        <v>303</v>
-      </c>
-      <c r="D38" s="40"/>
-      <c r="E38" s="41"/>
-      <c r="F38" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="G38" s="42"/>
-    </row>
-    <row r="39" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A39" s="39">
-        <v>11.4</v>
-      </c>
-      <c r="B39" s="21" t="s">
-        <v>242</v>
-      </c>
-      <c r="C39" s="40" t="s">
-        <v>246</v>
-      </c>
-      <c r="D39" s="40" t="s">
+      <c r="E39" s="38"/>
+      <c r="F39" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="G39" s="39"/>
+    </row>
+    <row r="40" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A40" s="36">
+        <v>11.41</v>
+      </c>
+      <c r="B40" s="18" t="s">
+        <v>239</v>
+      </c>
+      <c r="C40" s="37" t="s">
+        <v>301</v>
+      </c>
+      <c r="D40" s="37"/>
+      <c r="E40" s="38"/>
+      <c r="F40" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="G40" s="39"/>
+    </row>
+    <row r="41" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A41" s="36">
+        <v>11.5</v>
+      </c>
+      <c r="B41" s="18" t="s">
+        <v>298</v>
+      </c>
+      <c r="C41" s="37" t="s">
+        <v>299</v>
+      </c>
+      <c r="D41" s="37" t="s">
         <v>307</v>
       </c>
-      <c r="E39" s="41"/>
-      <c r="F39" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="G39" s="42"/>
-    </row>
-    <row r="40" spans="1:7" ht="68" x14ac:dyDescent="0.2">
-      <c r="A40" s="39">
-        <v>11.41</v>
-      </c>
-      <c r="B40" s="21" t="s">
-        <v>240</v>
-      </c>
-      <c r="C40" s="40" t="s">
-        <v>302</v>
-      </c>
-      <c r="D40" s="40"/>
-      <c r="E40" s="41"/>
-      <c r="F40" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="G40" s="42"/>
-    </row>
-    <row r="41" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A41" s="39">
-        <v>11.5</v>
-      </c>
-      <c r="B41" s="21" t="s">
-        <v>299</v>
-      </c>
-      <c r="C41" s="40" t="s">
+      <c r="E41" s="38"/>
+      <c r="F41" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="G41" s="39"/>
+    </row>
+    <row r="42" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A42" s="36">
+        <v>11.51</v>
+      </c>
+      <c r="B42" s="18" t="s">
+        <v>239</v>
+      </c>
+      <c r="C42" s="37" t="s">
         <v>300</v>
       </c>
-      <c r="D41" s="40" t="s">
+      <c r="D42" s="37"/>
+      <c r="E42" s="38"/>
+      <c r="F42" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="G42" s="39"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" s="35">
+        <v>12</v>
+      </c>
+      <c r="B43" s="28" t="s">
         <v>308</v>
       </c>
-      <c r="E41" s="41"/>
-      <c r="F41" s="22"/>
-      <c r="G41" s="42"/>
-    </row>
-    <row r="42" spans="1:7" ht="68" x14ac:dyDescent="0.2">
-      <c r="A42" s="39">
-        <v>11.51</v>
-      </c>
-      <c r="B42" s="21" t="s">
-        <v>240</v>
-      </c>
-      <c r="C42" s="40" t="s">
-        <v>301</v>
-      </c>
-      <c r="D42" s="40"/>
-      <c r="E42" s="41"/>
-      <c r="F42" s="22"/>
-      <c r="G42" s="42"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43" s="7">
-        <v>13</v>
-      </c>
-      <c r="B43" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="C43" s="8"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="9">
-        <v>44045</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C44" s="4"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C45" s="4"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C46" s="4"/>
+      <c r="C43" s="29"/>
+      <c r="D43" s="29"/>
+      <c r="E43" s="30"/>
+      <c r="F43" s="40"/>
+      <c r="G43" s="5"/>
+    </row>
+    <row r="44" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <v>12.01</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="D44" s="44" t="s">
+        <v>311</v>
+      </c>
+      <c r="F44" s="19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <v>12.02</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="D45" s="44" t="s">
+        <v>314</v>
+      </c>
+      <c r="F45" s="19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <v>12.03</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="D46" s="41" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C47" s="4"/>
@@ -2685,24 +2749,6 @@
     </row>
     <row r="121" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C121" s="4"/>
-    </row>
-    <row r="122" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C122" s="4"/>
-    </row>
-    <row r="123" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C123" s="4"/>
-    </row>
-    <row r="124" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C124" s="4"/>
-    </row>
-    <row r="125" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C125" s="4"/>
-    </row>
-    <row r="126" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C126" s="4"/>
-    </row>
-    <row r="127" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C127" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2711,6 +2757,7 @@
     <hyperlink ref="G7" r:id="rId3" xr:uid="{EC8665CB-F279-D846-A7CF-82110EFEED8C}"/>
     <hyperlink ref="G11:G15" r:id="rId4" display="https://git.generalassemb.ly/jdr-0622/sequelize-intro" xr:uid="{B69A30FC-A041-8243-8A0C-50F42F713089}"/>
     <hyperlink ref="G29" r:id="rId5" xr:uid="{ABA8700E-0CD3-B748-B3DC-647F717D4F03}"/>
+    <hyperlink ref="G34" r:id="rId6" xr:uid="{55755E6A-0B60-3C4B-931A-93F75C0FFA2C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2962,489 +3009,489 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="42" t="s">
+        <v>139</v>
+      </c>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+    </row>
+    <row r="3" spans="1:8" s="8" customFormat="1" ht="38" x14ac:dyDescent="0.2">
+      <c r="A3" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="61" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="G8" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-    </row>
-    <row r="3" spans="1:8" s="11" customFormat="1" ht="38" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
+      <c r="H8" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="57" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="7"/>
+    </row>
+    <row r="13" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="7"/>
+    </row>
+    <row r="14" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="43" t="s">
+        <v>147</v>
+      </c>
+      <c r="B14" s="43"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="43"/>
+    </row>
+    <row r="15" spans="1:8" ht="38" x14ac:dyDescent="0.2">
+      <c r="A15" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="B15" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="C15" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="G15" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="C3" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="H3" s="15" t="s">
+      <c r="H15" s="12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
+    <row r="16" spans="1:8" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A16" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="C16" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="G16" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="H16" s="14" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A17" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="G17" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="H17" s="14" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="18" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A18" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="G18" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="H4" s="10" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+      <c r="H18" s="14" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A19" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="F19" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="G19" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="H19" s="14" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="60" x14ac:dyDescent="0.2">
+      <c r="A20" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="B20" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="61" x14ac:dyDescent="0.2">
-      <c r="A8" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="G8" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="57" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="G9" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="H9" s="10" t="s">
+      <c r="C20" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="F20" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="G20" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="H20" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="A21" s="14" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="A10" s="10" t="s">
+      <c r="B21" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="B10" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="G10" s="18" t="s">
+      <c r="C21" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="H10" s="10" t="s">
+      <c r="D21" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="F21" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="G21" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="H21" s="14" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A22" s="14" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
+      <c r="B22" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="G11" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="H11" s="10" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="10"/>
-    </row>
-    <row r="13" spans="1:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="10"/>
-    </row>
-    <row r="14" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="46" t="s">
-        <v>148</v>
-      </c>
-      <c r="B14" s="46"/>
-      <c r="C14" s="46"/>
-      <c r="D14" s="46"/>
-      <c r="E14" s="46"/>
-      <c r="F14" s="46"/>
-      <c r="G14" s="46"/>
-      <c r="H14" s="46"/>
-    </row>
-    <row r="15" spans="1:8" ht="38" x14ac:dyDescent="0.2">
-      <c r="A15" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="F15" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="G15" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="H15" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A16" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="E16" s="17" t="s">
+      <c r="C22" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="E22" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="F16" s="20" t="s">
-        <v>169</v>
-      </c>
-      <c r="G16" s="20" t="s">
-        <v>149</v>
-      </c>
-      <c r="H16" s="17" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A17" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="E17" s="17" t="s">
-        <v>154</v>
-      </c>
-      <c r="F17" s="20" t="s">
-        <v>152</v>
-      </c>
-      <c r="G17" s="20" t="s">
-        <v>155</v>
-      </c>
-      <c r="H17" s="17" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" s="21" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A18" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="E18" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="F18" s="20" t="s">
-        <v>145</v>
-      </c>
-      <c r="G18" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="H18" s="17" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="A19" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="E19" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="F19" s="20" t="s">
-        <v>159</v>
-      </c>
-      <c r="G19" s="20" t="s">
-        <v>160</v>
-      </c>
-      <c r="H19" s="17" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="60" x14ac:dyDescent="0.2">
-      <c r="A20" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>147</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="E20" s="17" t="s">
+      <c r="F22" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="F20" s="20" t="s">
-        <v>162</v>
-      </c>
-      <c r="G20" s="20" t="s">
-        <v>155</v>
-      </c>
-      <c r="H20" s="17" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.2">
-      <c r="A21" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="B21" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="E21" s="17" t="s">
-        <v>154</v>
-      </c>
-      <c r="F21" s="20" t="s">
-        <v>159</v>
-      </c>
-      <c r="G21" s="20" t="s">
-        <v>165</v>
-      </c>
-      <c r="H21" s="17" t="s">
+      <c r="G22" s="17" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="A22" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="B22" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="E22" s="17" t="s">
-        <v>154</v>
-      </c>
-      <c r="F22" s="20" t="s">
-        <v>159</v>
-      </c>
-      <c r="G22" s="20" t="s">
+      <c r="H22" s="14" t="s">
         <v>167</v>
-      </c>
-      <c r="H22" s="17" t="s">
-        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -3477,835 +3524,835 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="24" t="s">
+        <v>171</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="H2" s="26" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="C3" s="20"/>
+      <c r="D3" s="31" t="s">
+        <v>179</v>
+      </c>
+      <c r="E3" s="31" t="s">
+        <v>178</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="G3" s="31" t="s">
+        <v>178</v>
+      </c>
+      <c r="H3" s="22"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="21" t="s">
+        <v>231</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="20"/>
+      <c r="D4" s="31" t="s">
+        <v>179</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="H4" s="22" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="C5" s="20">
+        <v>255</v>
+      </c>
+      <c r="D5" s="31" t="s">
+        <v>179</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="H5" s="22" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="21" t="s">
+        <v>232</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>186</v>
+      </c>
+      <c r="C6" s="20"/>
+      <c r="D6" s="31" t="s">
+        <v>179</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="H6" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="21" t="s">
+        <v>233</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="C7" s="20">
+        <v>255</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="H7" s="22"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="21" t="s">
+        <v>234</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="C8" s="20"/>
+      <c r="D8" s="31" t="s">
+        <v>179</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="F8" s="31" t="s">
+        <v>178</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="H8" s="22"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="21" t="s">
         <v>170</v>
       </c>
-      <c r="B1" s="26" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="27" t="s">
+      <c r="B9" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="C9" s="20"/>
+      <c r="D9" s="31" t="s">
+        <v>179</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="F9" s="31" t="s">
+        <v>178</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="H9" s="22"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="C10" s="20"/>
+      <c r="D10" s="31" t="s">
+        <v>179</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="F10" s="31" t="s">
+        <v>178</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="H10" s="22"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="21" t="s">
+        <v>250</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="C11" s="20"/>
+      <c r="D11" s="31" t="s">
+        <v>179</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="F11" s="31" t="s">
+        <v>178</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="H11" s="22"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="21" t="s">
+        <v>251</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="C12" s="20"/>
+      <c r="D12" s="31" t="s">
+        <v>179</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="F12" s="31" t="s">
+        <v>178</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="H12" s="22"/>
+    </row>
+    <row r="15" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="A15" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="24" t="s">
+        <v>171</v>
+      </c>
+      <c r="B16" s="25" t="s">
         <v>172</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="C16" s="25" t="s">
         <v>173</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="D16" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="E16" s="25" t="s">
         <v>174</v>
       </c>
-      <c r="D2" s="28" t="s">
-        <v>182</v>
-      </c>
-      <c r="E2" s="28" t="s">
+      <c r="F16" s="25" t="s">
         <v>175</v>
       </c>
-      <c r="F2" s="28" t="s">
+      <c r="G16" s="25" t="s">
         <v>176</v>
       </c>
-      <c r="G2" s="28" t="s">
+      <c r="H16" s="26" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="B17" s="20" t="s">
         <v>177</v>
       </c>
-      <c r="H2" s="29" t="s">
+      <c r="C17" s="20"/>
+      <c r="D17" s="31" t="s">
+        <v>179</v>
+      </c>
+      <c r="E17" s="31" t="s">
+        <v>178</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="G17" s="31" t="s">
+        <v>178</v>
+      </c>
+      <c r="H17" s="22"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="C18" s="20">
+        <v>255</v>
+      </c>
+      <c r="D18" s="31" t="s">
+        <v>179</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="G18" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="H18" s="22" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="21" t="s">
+        <v>217</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>219</v>
+      </c>
+      <c r="C19" s="20"/>
+      <c r="D19" s="31" t="s">
+        <v>179</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="F19" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="G19" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="H19" s="22" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="24" t="s">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="21" t="s">
+        <v>218</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>219</v>
+      </c>
+      <c r="C20" s="20"/>
+      <c r="D20" s="31" t="s">
+        <v>179</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="F20" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="G20" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="H20" s="22" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="A22" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="24" t="s">
+        <v>171</v>
+      </c>
+      <c r="B23" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="C23" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="D23" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="E23" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="F23" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="G23" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="H23" s="26" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="C24" s="20"/>
+      <c r="D24" s="31" t="s">
+        <v>179</v>
+      </c>
+      <c r="E24" s="31" t="s">
+        <v>178</v>
+      </c>
+      <c r="F24" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="G24" s="31" t="s">
+        <v>178</v>
+      </c>
+      <c r="H24" s="22"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="21" t="s">
         <v>196</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B25" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="C25" s="20">
+        <v>255</v>
+      </c>
+      <c r="D25" s="31" t="s">
+        <v>179</v>
+      </c>
+      <c r="E25" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="F25" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="G25" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="H25" s="22" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="21" t="s">
+        <v>217</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>219</v>
+      </c>
+      <c r="C26" s="20"/>
+      <c r="D26" s="31" t="s">
+        <v>179</v>
+      </c>
+      <c r="E26" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="F26" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="G26" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="H26" s="22" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="21" t="s">
+        <v>218</v>
+      </c>
+      <c r="B27" s="20" t="s">
+        <v>219</v>
+      </c>
+      <c r="C27" s="20"/>
+      <c r="D27" s="31" t="s">
+        <v>179</v>
+      </c>
+      <c r="E27" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="F27" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="G27" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="H27" s="22" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="A29" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="B29" s="23" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="24" t="s">
+        <v>171</v>
+      </c>
+      <c r="B30" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="C30" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="D30" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="E30" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="F30" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="G30" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="H30" s="26" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="B31" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="C31" s="20"/>
+      <c r="D31" s="31" t="s">
+        <v>179</v>
+      </c>
+      <c r="E31" s="31" t="s">
         <v>178</v>
       </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="34" t="s">
+      <c r="F31" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="G31" s="31" t="s">
+        <v>178</v>
+      </c>
+      <c r="H31" s="22"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="B32" s="20" t="s">
         <v>180</v>
       </c>
-      <c r="E3" s="34" t="s">
-        <v>179</v>
-      </c>
-      <c r="F3" s="23" t="s">
+      <c r="C32" s="20">
+        <v>255</v>
+      </c>
+      <c r="D32" s="31" t="s">
+        <v>179</v>
+      </c>
+      <c r="E32" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="F32" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="G32" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="H32" s="22" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="21" t="s">
+        <v>217</v>
+      </c>
+      <c r="B33" s="20" t="s">
+        <v>219</v>
+      </c>
+      <c r="C33" s="20"/>
+      <c r="D33" s="31" t="s">
+        <v>179</v>
+      </c>
+      <c r="E33" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="F33" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="G33" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="H33" s="22" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="21" t="s">
+        <v>218</v>
+      </c>
+      <c r="B34" s="20" t="s">
+        <v>219</v>
+      </c>
+      <c r="C34" s="20"/>
+      <c r="D34" s="31" t="s">
+        <v>179</v>
+      </c>
+      <c r="E34" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="F34" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="G34" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="H34" s="22" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="A36" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="B36" s="23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="24" t="s">
+        <v>171</v>
+      </c>
+      <c r="B37" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="C37" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="D37" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="E37" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="F37" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="G37" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="H37" s="26" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="B38" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="C38" s="20"/>
+      <c r="D38" s="31" t="s">
+        <v>179</v>
+      </c>
+      <c r="E38" s="31" t="s">
+        <v>178</v>
+      </c>
+      <c r="F38" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="G38" s="31" t="s">
+        <v>178</v>
+      </c>
+      <c r="H38" s="22"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="B39" s="20" t="s">
         <v>180</v>
       </c>
-      <c r="G3" s="34" t="s">
-        <v>179</v>
-      </c>
-      <c r="H3" s="25"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="24" t="s">
-        <v>232</v>
-      </c>
-      <c r="B4" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="34" t="s">
+      <c r="C39" s="20">
+        <v>255</v>
+      </c>
+      <c r="D39" s="31" t="s">
+        <v>179</v>
+      </c>
+      <c r="E39" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="F39" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="G39" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="H39" s="22" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="21" t="s">
+        <v>247</v>
+      </c>
+      <c r="B40" s="20" t="s">
         <v>180</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="C40" s="20">
+        <v>255</v>
+      </c>
+      <c r="D40" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="E40" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="F40" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="G40" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="H40" s="22"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="21" t="s">
+        <v>248</v>
+      </c>
+      <c r="B41" s="20" t="s">
         <v>180</v>
       </c>
-      <c r="F4" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="G4" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="H4" s="25" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="24" t="s">
-        <v>197</v>
-      </c>
-      <c r="B5" s="23" t="s">
-        <v>181</v>
-      </c>
-      <c r="C5" s="23">
+      <c r="C41" s="20">
         <v>255</v>
       </c>
-      <c r="D5" s="34" t="s">
-        <v>180</v>
-      </c>
-      <c r="E5" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="F5" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="G5" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="H5" s="25" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="24" t="s">
-        <v>233</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>187</v>
-      </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="34" t="s">
-        <v>180</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="F6" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="G6" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="H6" s="25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="24" t="s">
-        <v>234</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>181</v>
-      </c>
-      <c r="C7" s="23">
-        <v>255</v>
-      </c>
-      <c r="D7" s="23" t="s">
-        <v>179</v>
-      </c>
-      <c r="E7" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="F7" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="G7" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="H7" s="25"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="24" t="s">
-        <v>235</v>
-      </c>
-      <c r="B8" s="23" t="s">
+      <c r="D41" s="20" t="s">
         <v>178</v>
       </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="34" t="s">
-        <v>180</v>
-      </c>
-      <c r="E8" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="F8" s="34" t="s">
-        <v>179</v>
-      </c>
-      <c r="G8" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="H8" s="25"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="24" t="s">
-        <v>171</v>
-      </c>
-      <c r="B9" s="23" t="s">
-        <v>178</v>
-      </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="34" t="s">
-        <v>180</v>
-      </c>
-      <c r="E9" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="F9" s="34" t="s">
-        <v>179</v>
-      </c>
-      <c r="G9" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="H9" s="25"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="24" t="s">
-        <v>250</v>
-      </c>
-      <c r="B10" s="23" t="s">
-        <v>178</v>
-      </c>
-      <c r="C10" s="23"/>
-      <c r="D10" s="34" t="s">
-        <v>180</v>
-      </c>
-      <c r="E10" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="F10" s="34" t="s">
-        <v>179</v>
-      </c>
-      <c r="G10" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="H10" s="25"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="24" t="s">
-        <v>251</v>
-      </c>
-      <c r="B11" s="23" t="s">
-        <v>178</v>
-      </c>
-      <c r="C11" s="23"/>
-      <c r="D11" s="34" t="s">
-        <v>180</v>
-      </c>
-      <c r="E11" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="F11" s="34" t="s">
-        <v>179</v>
-      </c>
-      <c r="G11" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="H11" s="25"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="24" t="s">
-        <v>252</v>
-      </c>
-      <c r="B12" s="23" t="s">
-        <v>178</v>
-      </c>
-      <c r="C12" s="23"/>
-      <c r="D12" s="34" t="s">
-        <v>180</v>
-      </c>
-      <c r="E12" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="F12" s="34" t="s">
-        <v>179</v>
-      </c>
-      <c r="G12" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="H12" s="25"/>
-    </row>
-    <row r="15" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A15" s="26" t="s">
-        <v>170</v>
-      </c>
-      <c r="B15" s="26" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="27" t="s">
-        <v>172</v>
-      </c>
-      <c r="B16" s="28" t="s">
-        <v>173</v>
-      </c>
-      <c r="C16" s="28" t="s">
-        <v>174</v>
-      </c>
-      <c r="D16" s="28" t="s">
-        <v>182</v>
-      </c>
-      <c r="E16" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="F16" s="28" t="s">
-        <v>176</v>
-      </c>
-      <c r="G16" s="28" t="s">
-        <v>177</v>
-      </c>
-      <c r="H16" s="29" t="s">
+      <c r="E41" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="F41" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="G41" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="H41" s="22"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" s="21" t="s">
+        <v>217</v>
+      </c>
+      <c r="B42" s="20" t="s">
+        <v>219</v>
+      </c>
+      <c r="C42" s="20"/>
+      <c r="D42" s="31" t="s">
+        <v>179</v>
+      </c>
+      <c r="E42" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="F42" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="G42" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="H42" s="22" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="24" t="s">
-        <v>196</v>
-      </c>
-      <c r="B17" s="23" t="s">
-        <v>178</v>
-      </c>
-      <c r="C17" s="23"/>
-      <c r="D17" s="34" t="s">
-        <v>180</v>
-      </c>
-      <c r="E17" s="34" t="s">
-        <v>179</v>
-      </c>
-      <c r="F17" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="G17" s="34" t="s">
-        <v>179</v>
-      </c>
-      <c r="H17" s="25"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="24" t="s">
-        <v>197</v>
-      </c>
-      <c r="B18" s="23" t="s">
-        <v>181</v>
-      </c>
-      <c r="C18" s="23">
-        <v>255</v>
-      </c>
-      <c r="D18" s="34" t="s">
-        <v>180</v>
-      </c>
-      <c r="E18" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="F18" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="G18" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="H18" s="25" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="24" t="s">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" s="21" t="s">
         <v>218</v>
       </c>
-      <c r="B19" s="23" t="s">
-        <v>220</v>
-      </c>
-      <c r="C19" s="23"/>
-      <c r="D19" s="34" t="s">
-        <v>180</v>
-      </c>
-      <c r="E19" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="F19" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="G19" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="H19" s="25" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="24" t="s">
+      <c r="B43" s="20" t="s">
         <v>219</v>
       </c>
-      <c r="B20" s="23" t="s">
-        <v>220</v>
-      </c>
-      <c r="C20" s="23"/>
-      <c r="D20" s="34" t="s">
-        <v>180</v>
-      </c>
-      <c r="E20" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="F20" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="G20" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="H20" s="25" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A22" s="26" t="s">
-        <v>170</v>
-      </c>
-      <c r="B22" s="26" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="27" t="s">
-        <v>172</v>
-      </c>
-      <c r="B23" s="28" t="s">
-        <v>173</v>
-      </c>
-      <c r="C23" s="28" t="s">
-        <v>174</v>
-      </c>
-      <c r="D23" s="28" t="s">
-        <v>182</v>
-      </c>
-      <c r="E23" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="F23" s="28" t="s">
-        <v>176</v>
-      </c>
-      <c r="G23" s="28" t="s">
-        <v>177</v>
-      </c>
-      <c r="H23" s="29" t="s">
+      <c r="C43" s="20"/>
+      <c r="D43" s="31" t="s">
+        <v>179</v>
+      </c>
+      <c r="E43" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="F43" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="G43" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="H43" s="22" t="s">
         <v>188</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="24" t="s">
-        <v>196</v>
-      </c>
-      <c r="B24" s="23" t="s">
-        <v>178</v>
-      </c>
-      <c r="C24" s="23"/>
-      <c r="D24" s="34" t="s">
-        <v>180</v>
-      </c>
-      <c r="E24" s="34" t="s">
-        <v>179</v>
-      </c>
-      <c r="F24" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="G24" s="34" t="s">
-        <v>179</v>
-      </c>
-      <c r="H24" s="25"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="24" t="s">
-        <v>197</v>
-      </c>
-      <c r="B25" s="23" t="s">
-        <v>181</v>
-      </c>
-      <c r="C25" s="23">
-        <v>255</v>
-      </c>
-      <c r="D25" s="34" t="s">
-        <v>180</v>
-      </c>
-      <c r="E25" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="F25" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="G25" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="H25" s="25" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="24" t="s">
-        <v>218</v>
-      </c>
-      <c r="B26" s="23" t="s">
-        <v>220</v>
-      </c>
-      <c r="C26" s="23"/>
-      <c r="D26" s="34" t="s">
-        <v>180</v>
-      </c>
-      <c r="E26" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="F26" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="G26" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="H26" s="25" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="24" t="s">
-        <v>219</v>
-      </c>
-      <c r="B27" s="23" t="s">
-        <v>220</v>
-      </c>
-      <c r="C27" s="23"/>
-      <c r="D27" s="34" t="s">
-        <v>180</v>
-      </c>
-      <c r="E27" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="F27" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="G27" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="H27" s="25" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A29" s="26" t="s">
-        <v>170</v>
-      </c>
-      <c r="B29" s="26" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="27" t="s">
-        <v>172</v>
-      </c>
-      <c r="B30" s="28" t="s">
-        <v>173</v>
-      </c>
-      <c r="C30" s="28" t="s">
-        <v>174</v>
-      </c>
-      <c r="D30" s="28" t="s">
-        <v>182</v>
-      </c>
-      <c r="E30" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="F30" s="28" t="s">
-        <v>176</v>
-      </c>
-      <c r="G30" s="28" t="s">
-        <v>177</v>
-      </c>
-      <c r="H30" s="29" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="24" t="s">
-        <v>196</v>
-      </c>
-      <c r="B31" s="23" t="s">
-        <v>178</v>
-      </c>
-      <c r="C31" s="23"/>
-      <c r="D31" s="34" t="s">
-        <v>180</v>
-      </c>
-      <c r="E31" s="34" t="s">
-        <v>179</v>
-      </c>
-      <c r="F31" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="G31" s="34" t="s">
-        <v>179</v>
-      </c>
-      <c r="H31" s="25"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="24" t="s">
-        <v>197</v>
-      </c>
-      <c r="B32" s="23" t="s">
-        <v>181</v>
-      </c>
-      <c r="C32" s="23">
-        <v>255</v>
-      </c>
-      <c r="D32" s="34" t="s">
-        <v>180</v>
-      </c>
-      <c r="E32" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="F32" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="G32" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="H32" s="25" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="24" t="s">
-        <v>218</v>
-      </c>
-      <c r="B33" s="23" t="s">
-        <v>220</v>
-      </c>
-      <c r="C33" s="23"/>
-      <c r="D33" s="34" t="s">
-        <v>180</v>
-      </c>
-      <c r="E33" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="F33" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="G33" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="H33" s="25" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="24" t="s">
-        <v>219</v>
-      </c>
-      <c r="B34" s="23" t="s">
-        <v>220</v>
-      </c>
-      <c r="C34" s="23"/>
-      <c r="D34" s="34" t="s">
-        <v>180</v>
-      </c>
-      <c r="E34" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="F34" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="G34" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="H34" s="25" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A36" s="26" t="s">
-        <v>170</v>
-      </c>
-      <c r="B36" s="26" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="27" t="s">
-        <v>172</v>
-      </c>
-      <c r="B37" s="28" t="s">
-        <v>173</v>
-      </c>
-      <c r="C37" s="28" t="s">
-        <v>174</v>
-      </c>
-      <c r="D37" s="28" t="s">
-        <v>182</v>
-      </c>
-      <c r="E37" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="F37" s="28" t="s">
-        <v>176</v>
-      </c>
-      <c r="G37" s="28" t="s">
-        <v>177</v>
-      </c>
-      <c r="H37" s="29" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="24" t="s">
-        <v>196</v>
-      </c>
-      <c r="B38" s="23" t="s">
-        <v>178</v>
-      </c>
-      <c r="C38" s="23"/>
-      <c r="D38" s="34" t="s">
-        <v>180</v>
-      </c>
-      <c r="E38" s="34" t="s">
-        <v>179</v>
-      </c>
-      <c r="F38" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="G38" s="34" t="s">
-        <v>179</v>
-      </c>
-      <c r="H38" s="25"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="24" t="s">
-        <v>197</v>
-      </c>
-      <c r="B39" s="23" t="s">
-        <v>181</v>
-      </c>
-      <c r="C39" s="23">
-        <v>255</v>
-      </c>
-      <c r="D39" s="34" t="s">
-        <v>180</v>
-      </c>
-      <c r="E39" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="F39" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="G39" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="H39" s="25" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="24" t="s">
-        <v>248</v>
-      </c>
-      <c r="B40" s="23" t="s">
-        <v>181</v>
-      </c>
-      <c r="C40" s="23">
-        <v>255</v>
-      </c>
-      <c r="D40" s="23" t="s">
-        <v>179</v>
-      </c>
-      <c r="E40" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="F40" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="G40" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="H40" s="25"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="24" t="s">
-        <v>249</v>
-      </c>
-      <c r="B41" s="23" t="s">
-        <v>181</v>
-      </c>
-      <c r="C41" s="23">
-        <v>255</v>
-      </c>
-      <c r="D41" s="23" t="s">
-        <v>179</v>
-      </c>
-      <c r="E41" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="F41" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="G41" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="H41" s="25"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A42" s="24" t="s">
-        <v>218</v>
-      </c>
-      <c r="B42" s="23" t="s">
-        <v>220</v>
-      </c>
-      <c r="C42" s="23"/>
-      <c r="D42" s="34" t="s">
-        <v>180</v>
-      </c>
-      <c r="E42" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="F42" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="G42" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="H42" s="25" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A43" s="24" t="s">
-        <v>219</v>
-      </c>
-      <c r="B43" s="23" t="s">
-        <v>220</v>
-      </c>
-      <c r="C43" s="23"/>
-      <c r="D43" s="34" t="s">
-        <v>180</v>
-      </c>
-      <c r="E43" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="F43" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="G43" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="H43" s="25" t="s">
-        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -4337,310 +4384,310 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:2" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="24" t="s">
+        <v>195</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="21">
+        <v>1</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="21">
+        <v>2</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="21">
+        <v>3</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="21">
+        <v>4</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="21">
+        <v>5</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="A10" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="24" t="s">
+        <v>195</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="21">
+        <v>1</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="21">
+        <v>2</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="21">
+        <v>3</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="21">
+        <v>4</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="21">
+        <v>5</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="21">
+        <v>6</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="21">
+        <v>7</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="21">
+        <v>8</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="32"/>
+      <c r="B20" s="32"/>
+    </row>
+    <row r="21" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A21" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="24" t="s">
+        <v>195</v>
+      </c>
+      <c r="B22" s="25" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="21">
+        <v>1</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="21">
+        <v>2</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="21">
+        <v>3</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="21">
+        <v>4</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="21">
+        <v>5</v>
+      </c>
+      <c r="B27" s="20" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="32"/>
+      <c r="B28" s="32"/>
+    </row>
+    <row r="29" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A29" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="B29" s="23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="24" t="s">
+        <v>195</v>
+      </c>
+      <c r="B30" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="C30" s="25" t="s">
+        <v>247</v>
+      </c>
+      <c r="D30" s="25" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="21">
+        <v>1</v>
+      </c>
+      <c r="B31" s="20" t="s">
+        <v>277</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>275</v>
+      </c>
+      <c r="D31" s="20" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="21">
+        <v>2</v>
+      </c>
+      <c r="B32" s="20" t="s">
+        <v>271</v>
+      </c>
+      <c r="C32" s="20" t="s">
+        <v>272</v>
+      </c>
+      <c r="D32" s="20" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+      <c r="A34" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="B34" s="23" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" s="24" t="s">
+        <v>195</v>
+      </c>
+      <c r="B35" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="C35" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="D35" s="25" t="s">
+        <v>232</v>
+      </c>
+      <c r="E35" s="25" t="s">
+        <v>233</v>
+      </c>
+      <c r="F35" s="25" t="s">
+        <v>234</v>
+      </c>
+      <c r="G35" s="25" t="s">
         <v>170</v>
       </c>
-      <c r="B2" s="26" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="27" t="s">
-        <v>196</v>
-      </c>
-      <c r="B3" s="28" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="24">
-        <v>1</v>
-      </c>
-      <c r="B4" s="23" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="24">
-        <v>2</v>
-      </c>
-      <c r="B5" s="23" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="24">
-        <v>3</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="24">
-        <v>4</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="24">
-        <v>5</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="21" x14ac:dyDescent="0.25">
-      <c r="A10" s="26" t="s">
-        <v>170</v>
-      </c>
-      <c r="B10" s="26" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="27" t="s">
-        <v>196</v>
-      </c>
-      <c r="B11" s="28" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="24">
-        <v>1</v>
-      </c>
-      <c r="B12" s="23" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="24">
-        <v>2</v>
-      </c>
-      <c r="B13" s="23" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="24">
-        <v>3</v>
-      </c>
-      <c r="B14" s="23" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="24">
-        <v>4</v>
-      </c>
-      <c r="B15" s="23" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="24">
-        <v>5</v>
-      </c>
-      <c r="B16" s="23" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="24">
-        <v>6</v>
-      </c>
-      <c r="B17" s="23" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="24">
-        <v>7</v>
-      </c>
-      <c r="B18" s="23" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="24">
-        <v>8</v>
-      </c>
-      <c r="B19" s="23" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="35"/>
-      <c r="B20" s="35"/>
-    </row>
-    <row r="21" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A21" s="26" t="s">
-        <v>170</v>
-      </c>
-      <c r="B21" s="26" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="27" t="s">
-        <v>196</v>
-      </c>
-      <c r="B22" s="28" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="24">
-        <v>1</v>
-      </c>
-      <c r="B23" s="23" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="24">
-        <v>2</v>
-      </c>
-      <c r="B24" s="23" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="24">
-        <v>3</v>
-      </c>
-      <c r="B25" s="23" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="24">
-        <v>4</v>
-      </c>
-      <c r="B26" s="23" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="24">
-        <v>5</v>
-      </c>
-      <c r="B27" s="23" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="35"/>
-      <c r="B28" s="35"/>
-    </row>
-    <row r="29" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A29" s="26" t="s">
-        <v>170</v>
-      </c>
-      <c r="B29" s="26" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="27" t="s">
-        <v>196</v>
-      </c>
-      <c r="B30" s="28" t="s">
-        <v>197</v>
-      </c>
-      <c r="C30" s="28" t="s">
-        <v>248</v>
-      </c>
-      <c r="D30" s="28" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="24">
-        <v>1</v>
-      </c>
-      <c r="B31" s="23" t="s">
-        <v>278</v>
-      </c>
-      <c r="C31" s="23" t="s">
-        <v>276</v>
-      </c>
-      <c r="D31" s="23" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="24">
-        <v>2</v>
-      </c>
-      <c r="B32" s="23" t="s">
-        <v>272</v>
-      </c>
-      <c r="C32" s="23" t="s">
-        <v>273</v>
-      </c>
-      <c r="D32" s="23" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="A34" s="26" t="s">
-        <v>170</v>
-      </c>
-      <c r="B34" s="26" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A35" s="27" t="s">
-        <v>196</v>
-      </c>
-      <c r="B35" s="28" t="s">
-        <v>232</v>
-      </c>
-      <c r="C35" s="28" t="s">
-        <v>197</v>
-      </c>
-      <c r="D35" s="28" t="s">
-        <v>233</v>
-      </c>
-      <c r="E35" s="28" t="s">
-        <v>234</v>
-      </c>
-      <c r="F35" s="28" t="s">
-        <v>235</v>
-      </c>
-      <c r="G35" s="28" t="s">
-        <v>171</v>
-      </c>
-      <c r="H35" s="28" t="s">
+      <c r="H35" s="25" t="s">
+        <v>249</v>
+      </c>
+      <c r="I35" s="25" t="s">
         <v>250</v>
       </c>
-      <c r="I35" s="28" t="s">
+      <c r="J35" s="25" t="s">
         <v>251</v>
-      </c>
-      <c r="J35" s="28" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>1</v>
       </c>
-      <c r="B36" s="44" t="s">
-        <v>290</v>
+      <c r="B36" s="41" t="s">
+        <v>289</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D36" s="36">
+        <v>279</v>
+      </c>
+      <c r="D36" s="33">
         <v>120</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F36" s="1">
         <v>1</v>
@@ -4662,13 +4709,13 @@
       <c r="A37" s="1">
         <v>2</v>
       </c>
-      <c r="B37" s="44" t="s">
-        <v>291</v>
+      <c r="B37" s="41" t="s">
+        <v>290</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="D37" s="36">
+        <v>280</v>
+      </c>
+      <c r="D37" s="33">
         <v>20</v>
       </c>
       <c r="F37" s="1">
@@ -4691,13 +4738,13 @@
       <c r="A38" s="1">
         <v>3</v>
       </c>
-      <c r="B38" s="44" t="s">
-        <v>291</v>
+      <c r="B38" s="41" t="s">
+        <v>290</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D38" s="36">
+        <v>281</v>
+      </c>
+      <c r="D38" s="33">
         <v>40</v>
       </c>
       <c r="F38" s="1">
@@ -4720,13 +4767,13 @@
       <c r="A39" s="1">
         <v>4</v>
       </c>
-      <c r="B39" s="44" t="s">
-        <v>292</v>
+      <c r="B39" s="41" t="s">
+        <v>291</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="D39" s="36">
+        <v>282</v>
+      </c>
+      <c r="D39" s="33">
         <v>150</v>
       </c>
       <c r="F39" s="1">
@@ -4749,13 +4796,13 @@
       <c r="A40" s="1">
         <v>5</v>
       </c>
-      <c r="B40" s="44" t="s">
-        <v>292</v>
+      <c r="B40" s="41" t="s">
+        <v>291</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="D40" s="36">
+        <v>283</v>
+      </c>
+      <c r="D40" s="33">
         <v>20</v>
       </c>
       <c r="F40" s="1">
@@ -4778,17 +4825,17 @@
       <c r="A41" s="1">
         <v>6</v>
       </c>
-      <c r="B41" s="44" t="s">
-        <v>292</v>
+      <c r="B41" s="41" t="s">
+        <v>291</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D41" s="36">
+        <v>284</v>
+      </c>
+      <c r="D41" s="33">
         <v>80.5</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F41" s="1">
         <v>1</v>
@@ -4810,17 +4857,17 @@
       <c r="A42" s="1">
         <v>7</v>
       </c>
-      <c r="B42" s="44" t="s">
-        <v>279</v>
+      <c r="B42" s="41" t="s">
+        <v>278</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D42" s="36">
+        <v>285</v>
+      </c>
+      <c r="D42" s="33">
         <v>500</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F42" s="1">
         <v>1</v>
@@ -4842,17 +4889,17 @@
       <c r="A43" s="1">
         <v>8</v>
       </c>
-      <c r="B43" s="44" t="s">
-        <v>293</v>
+      <c r="B43" s="41" t="s">
+        <v>292</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="D43" s="36">
+        <v>286</v>
+      </c>
+      <c r="D43" s="33">
         <v>300</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F43" s="1">
         <v>1</v>
@@ -4874,17 +4921,17 @@
       <c r="A44" s="1">
         <v>9</v>
       </c>
-      <c r="B44" s="44" t="s">
-        <v>293</v>
+      <c r="B44" s="41" t="s">
+        <v>292</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="D44" s="36">
+        <v>287</v>
+      </c>
+      <c r="D44" s="33">
         <v>800</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F44" s="1">
         <v>1</v>
@@ -4906,13 +4953,13 @@
       <c r="A45" s="1">
         <v>10</v>
       </c>
-      <c r="B45" s="44" t="s">
-        <v>294</v>
+      <c r="B45" s="41" t="s">
+        <v>293</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="D45" s="36">
+        <v>288</v>
+      </c>
+      <c r="D45" s="33">
         <v>120</v>
       </c>
       <c r="F45" s="1">
@@ -4940,7 +4987,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFD95FFD-3F78-284D-BA72-713E3F9CEBC1}">
   <dimension ref="A2:B24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>

</xml_diff>